<commit_message>
Inicio sprite jefe vampiro
</commit_message>
<xml_diff>
--- a/doc/diseño sprites/diseno sprites.xlsx
+++ b/doc/diseño sprites/diseno sprites.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="zombi" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="fuego" sheetId="4" r:id="rId4"/>
     <sheet name="fantasma" sheetId="5" r:id="rId5"/>
     <sheet name="magia" sheetId="6" r:id="rId6"/>
+    <sheet name="jefevampiro" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="254">
   <si>
     <t>00011111n</t>
   </si>
@@ -770,6 +771,27 @@
   </si>
   <si>
     <t>n00111010</t>
+  </si>
+  <si>
+    <t>n11101011</t>
+  </si>
+  <si>
+    <t>n11111001</t>
+  </si>
+  <si>
+    <t>n11110001</t>
+  </si>
+  <si>
+    <t>n00111011</t>
+  </si>
+  <si>
+    <t>n10001111</t>
+  </si>
+  <si>
+    <t>n11010111</t>
+  </si>
+  <si>
+    <t>n11110011</t>
   </si>
 </sst>
 </file>
@@ -8762,8 +8784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:P16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -9699,4 +9721,467 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E2" t="s">
+        <v>156</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E3" t="s">
+        <v>233</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>237</v>
+      </c>
+      <c r="E4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>237</v>
+      </c>
+      <c r="E6" t="s">
+        <v>152</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>237</v>
+      </c>
+      <c r="E7" t="s">
+        <v>152</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>208</v>
+      </c>
+      <c r="E12" t="s">
+        <v>236</v>
+      </c>
+      <c r="F12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>247</v>
+      </c>
+      <c r="E13" t="s">
+        <v>252</v>
+      </c>
+      <c r="F13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" t="s">
+        <v>216</v>
+      </c>
+      <c r="B16" t="s">
+        <v>82</v>
+      </c>
+      <c r="E16" t="s">
+        <v>80</v>
+      </c>
+      <c r="F16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" t="s">
+        <v>250</v>
+      </c>
+      <c r="E18" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>147</v>
+      </c>
+      <c r="B19" t="s">
+        <v>153</v>
+      </c>
+      <c r="E19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" t="s">
+        <v>7</v>
+      </c>
+      <c r="F21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="E23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" t="s">
+        <v>208</v>
+      </c>
+      <c r="E25" t="s">
+        <v>236</v>
+      </c>
+      <c r="F25" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" t="s">
+        <v>148</v>
+      </c>
+      <c r="E26" t="s">
+        <v>253</v>
+      </c>
+      <c r="F26" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>152</v>
+      </c>
+      <c r="B27" t="s">
+        <v>251</v>
+      </c>
+      <c r="E27" t="s">
+        <v>249</v>
+      </c>
+      <c r="F27" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>248</v>
+      </c>
+      <c r="B28" t="s">
+        <v>71</v>
+      </c>
+      <c r="E28" t="s">
+        <v>249</v>
+      </c>
+      <c r="F28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>249</v>
+      </c>
+      <c r="B29" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" t="s">
+        <v>33</v>
+      </c>
+      <c r="F29" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>169</v>
+      </c>
+      <c r="B30" t="s">
+        <v>11</v>
+      </c>
+      <c r="E30" t="s">
+        <v>76</v>
+      </c>
+      <c r="F30" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>169</v>
+      </c>
+      <c r="B31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" t="s">
+        <v>101</v>
+      </c>
+      <c r="F31" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" t="s">
+        <v>3</v>
+      </c>
+      <c r="F33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fin sprite jefe vampiro
</commit_message>
<xml_diff>
--- a/doc/diseño sprites/diseno sprites.xlsx
+++ b/doc/diseño sprites/diseno sprites.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="254">
   <si>
     <t>00011111n</t>
   </si>
@@ -8785,7 +8785,7 @@
   <dimension ref="A1:P16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -9725,449 +9725,1813 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P17" sqref="O17:P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>3</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
+      <c r="C1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(A1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="D1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(B1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(E1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="H1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(F1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(I1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="L1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(J1,1,1,""),2))</f>
+        <v>#20</v>
+      </c>
+      <c r="M1" t="s">
+        <v>216</v>
+      </c>
+      <c r="N1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(M1,1,1,""),2))</f>
+        <v>#04</v>
+      </c>
+      <c r="P1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(N1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>169</v>
       </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C32" si="0">CONCATENATE("#",BIN2HEX(REPLACE(A2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D32" si="1">CONCATENATE("#",BIN2HEX(REPLACE(B2,1,1,""),2))</f>
+        <v>#60</v>
+      </c>
       <c r="E2" t="s">
         <v>156</v>
       </c>
       <c r="F2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G33" si="2">CONCATENATE("#",BIN2HEX(REPLACE(E2,1,1,""),2))</f>
+        <v>#06</v>
+      </c>
+      <c r="H2" t="str">
+        <f t="shared" ref="H2:H33" si="3">CONCATENATE("#",BIN2HEX(REPLACE(F2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" t="s">
+        <v>169</v>
+      </c>
+      <c r="K2" t="str">
+        <f t="shared" ref="K2:K33" si="4">CONCATENATE("#",BIN2HEX(REPLACE(I2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="L2" t="str">
+        <f t="shared" ref="L2:L33" si="5">CONCATENATE("#",BIN2HEX(REPLACE(J2,1,1,""),2))</f>
+        <v>#60</v>
+      </c>
+      <c r="M2" t="s">
+        <v>156</v>
+      </c>
+      <c r="N2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" t="str">
+        <f t="shared" ref="O2:O33" si="6">CONCATENATE("#",BIN2HEX(REPLACE(M2,1,1,""),2))</f>
+        <v>#06</v>
+      </c>
+      <c r="P2" t="str">
+        <f t="shared" ref="P2:P33" si="7">CONCATENATE("#",BIN2HEX(REPLACE(N2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>232</v>
       </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="1"/>
+        <v>#90</v>
+      </c>
       <c r="E3" t="s">
         <v>233</v>
       </c>
       <c r="F3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3" t="str">
+        <f t="shared" si="2"/>
+        <v>#09</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>232</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" si="5"/>
+        <v>#90</v>
+      </c>
+      <c r="M3" t="s">
+        <v>233</v>
+      </c>
+      <c r="N3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3" t="str">
+        <f t="shared" si="6"/>
+        <v>#09</v>
+      </c>
+      <c r="P3" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>237</v>
       </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v>#BF</v>
+      </c>
       <c r="E4" t="s">
         <v>152</v>
       </c>
       <c r="F4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4" t="str">
+        <f t="shared" si="2"/>
+        <v>#FD</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>237</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="5"/>
+        <v>#BF</v>
+      </c>
+      <c r="M4" t="s">
+        <v>152</v>
+      </c>
+      <c r="N4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O4" t="str">
+        <f t="shared" si="6"/>
+        <v>#FD</v>
+      </c>
+      <c r="P4" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>35</v>
       </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
       <c r="E5" t="s">
         <v>35</v>
       </c>
       <c r="F5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M5" t="s">
+        <v>35</v>
+      </c>
+      <c r="N5" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P5" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>237</v>
       </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="1"/>
+        <v>#BF</v>
+      </c>
       <c r="E6" t="s">
         <v>152</v>
       </c>
       <c r="F6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6" t="str">
+        <f t="shared" si="2"/>
+        <v>#FD</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" t="s">
+        <v>237</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="5"/>
+        <v>#BF</v>
+      </c>
+      <c r="M6" t="s">
+        <v>152</v>
+      </c>
+      <c r="N6" t="s">
+        <v>3</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" si="6"/>
+        <v>#FD</v>
+      </c>
+      <c r="P6" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7" t="s">
         <v>237</v>
       </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="1"/>
+        <v>#BF</v>
+      </c>
       <c r="E7" t="s">
         <v>152</v>
       </c>
       <c r="F7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7" t="str">
+        <f t="shared" si="2"/>
+        <v>#FD</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" t="s">
+        <v>237</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="5"/>
+        <v>#BF</v>
+      </c>
+      <c r="M7" t="s">
+        <v>152</v>
+      </c>
+      <c r="N7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="6"/>
+        <v>#FD</v>
+      </c>
+      <c r="P7" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8" t="s">
         <v>35</v>
       </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
       <c r="E8" t="s">
         <v>35</v>
       </c>
       <c r="F8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" t="s">
+        <v>35</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M8" t="s">
+        <v>35</v>
+      </c>
+      <c r="N8" t="s">
+        <v>3</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>3</v>
       </c>
       <c r="B9" t="s">
         <v>37</v>
       </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="1"/>
+        <v>#7F</v>
+      </c>
       <c r="E9" t="s">
         <v>14</v>
       </c>
       <c r="F9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="G9" t="str">
+        <f t="shared" si="2"/>
+        <v>#FE</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" t="s">
+        <v>37</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="5"/>
+        <v>#7F</v>
+      </c>
+      <c r="M9" t="s">
+        <v>14</v>
+      </c>
+      <c r="N9" t="s">
+        <v>3</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="6"/>
+        <v>#FE</v>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
         <v>3</v>
       </c>
       <c r="B10" t="s">
         <v>35</v>
       </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
       <c r="E10" t="s">
         <v>35</v>
       </c>
       <c r="F10" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="G10" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" t="s">
+        <v>35</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M10" t="s">
+        <v>35</v>
+      </c>
+      <c r="N10" t="s">
+        <v>3</v>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P10" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
         <v>3</v>
       </c>
       <c r="B11" t="s">
         <v>35</v>
       </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
       <c r="E11" t="s">
         <v>35</v>
       </c>
       <c r="F11" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="G11" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I11" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" t="s">
+        <v>208</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="5"/>
+        <v>#EF</v>
+      </c>
+      <c r="M11" t="s">
+        <v>236</v>
+      </c>
+      <c r="N11" t="s">
+        <v>3</v>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" si="6"/>
+        <v>#F7</v>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>3</v>
       </c>
       <c r="B12" t="s">
         <v>208</v>
       </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v>#EF</v>
+      </c>
       <c r="E12" t="s">
         <v>236</v>
       </c>
       <c r="F12" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="G12" t="str">
+        <f t="shared" si="2"/>
+        <v>#F7</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I12" t="s">
+        <v>3</v>
+      </c>
+      <c r="J12" t="s">
+        <v>154</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="5"/>
+        <v>#E3</v>
+      </c>
+      <c r="M12" t="s">
+        <v>94</v>
+      </c>
+      <c r="N12" t="s">
+        <v>3</v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" si="6"/>
+        <v>#C7</v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13" t="s">
         <v>3</v>
       </c>
       <c r="B13" t="s">
         <v>247</v>
       </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v>#EB</v>
+      </c>
       <c r="E13" t="s">
         <v>252</v>
       </c>
       <c r="F13" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="G13" t="str">
+        <f t="shared" si="2"/>
+        <v>#D7</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I13" t="s">
+        <v>216</v>
+      </c>
+      <c r="J13" t="s">
+        <v>35</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="4"/>
+        <v>#04</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M13" t="s">
+        <v>35</v>
+      </c>
+      <c r="N13" t="s">
+        <v>55</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P13" t="str">
+        <f t="shared" si="7"/>
+        <v>#20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
         <v>3</v>
       </c>
       <c r="B14" t="s">
         <v>35</v>
       </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
       <c r="E14" t="s">
         <v>35</v>
       </c>
       <c r="F14" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="G14" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I14" t="s">
+        <v>65</v>
+      </c>
+      <c r="J14" t="s">
+        <v>35</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="4"/>
+        <v>#0E</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M14" t="s">
+        <v>35</v>
+      </c>
+      <c r="N14" t="s">
+        <v>30</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P14" t="str">
+        <f t="shared" si="7"/>
+        <v>#70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15" t="s">
         <v>3</v>
       </c>
       <c r="B15" t="s">
         <v>37</v>
       </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>#7F</v>
+      </c>
       <c r="E15" t="s">
         <v>14</v>
       </c>
       <c r="F15" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="G15" t="str">
+        <f t="shared" si="2"/>
+        <v>#FE</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I15" t="s">
+        <v>147</v>
+      </c>
+      <c r="J15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="4"/>
+        <v>#1E</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="5"/>
+        <v>#78</v>
+      </c>
+      <c r="M15" t="s">
+        <v>147</v>
+      </c>
+      <c r="N15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O15" t="str">
+        <f t="shared" si="6"/>
+        <v>#1E</v>
+      </c>
+      <c r="P15" t="str">
+        <f t="shared" si="7"/>
+        <v>#78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="A16" t="s">
         <v>216</v>
       </c>
       <c r="B16" t="s">
         <v>82</v>
       </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>#04</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>#7C</v>
+      </c>
       <c r="E16" t="s">
         <v>80</v>
       </c>
       <c r="F16" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G16" t="str">
+        <f t="shared" si="2"/>
+        <v>#3E</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="3"/>
+        <v>#20</v>
+      </c>
+      <c r="I16" t="s">
+        <v>43</v>
+      </c>
+      <c r="J16" t="s">
+        <v>204</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="4"/>
+        <v>#3F</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="5"/>
+        <v>#7B</v>
+      </c>
+      <c r="M16" t="s">
+        <v>207</v>
+      </c>
+      <c r="N16" t="s">
+        <v>7</v>
+      </c>
+      <c r="O16" t="str">
+        <f t="shared" si="6"/>
+        <v>#DE</v>
+      </c>
+      <c r="P16" t="str">
+        <f t="shared" si="7"/>
+        <v>#FC</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
       <c r="A18" t="s">
         <v>65</v>
       </c>
       <c r="B18" t="s">
         <v>250</v>
       </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>#0E</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="1"/>
+        <v>#3B</v>
+      </c>
       <c r="E18" t="s">
         <v>57</v>
       </c>
       <c r="F18" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18" t="str">
+        <f t="shared" si="2"/>
+        <v>#DC</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="3"/>
+        <v>#70</v>
+      </c>
+      <c r="I18" t="s">
+        <v>43</v>
+      </c>
+      <c r="J18" t="s">
+        <v>43</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="4"/>
+        <v>#3F</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="5"/>
+        <v>#3F</v>
+      </c>
+      <c r="M18" t="s">
+        <v>7</v>
+      </c>
+      <c r="N18" t="s">
+        <v>7</v>
+      </c>
+      <c r="O18" t="str">
+        <f t="shared" si="6"/>
+        <v>#FC</v>
+      </c>
+      <c r="P18" t="str">
+        <f t="shared" si="7"/>
+        <v>#FC</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19" t="s">
         <v>147</v>
       </c>
       <c r="B19" t="s">
         <v>153</v>
       </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>#1E</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="1"/>
+        <v>#1F</v>
+      </c>
       <c r="E19" t="s">
         <v>2</v>
       </c>
       <c r="F19" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19" t="str">
+        <f t="shared" si="2"/>
+        <v>#F8</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="3"/>
+        <v>#78</v>
+      </c>
+      <c r="I19" t="s">
+        <v>43</v>
+      </c>
+      <c r="J19" t="s">
+        <v>153</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="4"/>
+        <v>#3F</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="5"/>
+        <v>#1F</v>
+      </c>
+      <c r="M19" t="s">
+        <v>2</v>
+      </c>
+      <c r="N19" t="s">
+        <v>7</v>
+      </c>
+      <c r="O19" t="str">
+        <f t="shared" si="6"/>
+        <v>#F8</v>
+      </c>
+      <c r="P19" t="str">
+        <f t="shared" si="7"/>
+        <v>#FC</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20" t="s">
         <v>43</v>
       </c>
       <c r="B20" t="s">
         <v>71</v>
       </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>#3F</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="1"/>
+        <v>#0F</v>
+      </c>
       <c r="E20" t="s">
         <v>9</v>
       </c>
       <c r="F20" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="G20" t="str">
+        <f t="shared" si="2"/>
+        <v>#F0</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="3"/>
+        <v>#FC</v>
+      </c>
+      <c r="I20" t="s">
+        <v>37</v>
+      </c>
+      <c r="J20" t="s">
+        <v>71</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="4"/>
+        <v>#7F</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="5"/>
+        <v>#0F</v>
+      </c>
+      <c r="M20" t="s">
+        <v>9</v>
+      </c>
+      <c r="N20" t="s">
+        <v>14</v>
+      </c>
+      <c r="O20" t="str">
+        <f t="shared" si="6"/>
+        <v>#F0</v>
+      </c>
+      <c r="P20" t="str">
+        <f t="shared" si="7"/>
+        <v>#FE</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
       <c r="A21" t="s">
         <v>43</v>
       </c>
       <c r="B21" t="s">
         <v>43</v>
       </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>#3F</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="1"/>
+        <v>#3F</v>
+      </c>
       <c r="E21" t="s">
         <v>7</v>
       </c>
       <c r="F21" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="G21" t="str">
+        <f t="shared" si="2"/>
+        <v>#FC</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="3"/>
+        <v>#FC</v>
+      </c>
+      <c r="I21" t="s">
+        <v>37</v>
+      </c>
+      <c r="J21" t="s">
+        <v>43</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="4"/>
+        <v>#7F</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="5"/>
+        <v>#3F</v>
+      </c>
+      <c r="M21" t="s">
+        <v>7</v>
+      </c>
+      <c r="N21" t="s">
+        <v>14</v>
+      </c>
+      <c r="O21" t="str">
+        <f t="shared" si="6"/>
+        <v>#FC</v>
+      </c>
+      <c r="P21" t="str">
+        <f t="shared" si="7"/>
+        <v>#FE</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
       <c r="A22" t="s">
         <v>43</v>
       </c>
       <c r="B22" t="s">
         <v>35</v>
       </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>#3F</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
       <c r="E22" t="s">
         <v>35</v>
       </c>
       <c r="F22" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="3"/>
+        <v>#FC</v>
+      </c>
+      <c r="I22" t="s">
+        <v>37</v>
+      </c>
+      <c r="J22" t="s">
+        <v>35</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="4"/>
+        <v>#7F</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M22" t="s">
+        <v>35</v>
+      </c>
+      <c r="N22" t="s">
+        <v>14</v>
+      </c>
+      <c r="O22" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P22" t="str">
+        <f t="shared" si="7"/>
+        <v>#FE</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23" t="s">
         <v>37</v>
       </c>
       <c r="B23" t="s">
         <v>35</v>
       </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>#7F</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
       <c r="E23" t="s">
         <v>35</v>
       </c>
       <c r="F23" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="3"/>
+        <v>#FE</v>
+      </c>
+      <c r="I23" t="s">
+        <v>35</v>
+      </c>
+      <c r="J23" t="s">
+        <v>35</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="4"/>
+        <v>#FF</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M23" t="s">
+        <v>35</v>
+      </c>
+      <c r="N23" t="s">
+        <v>35</v>
+      </c>
+      <c r="O23" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P23" t="str">
+        <f t="shared" si="7"/>
+        <v>#FF</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
       <c r="A24" t="s">
         <v>37</v>
       </c>
       <c r="B24" t="s">
         <v>35</v>
       </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>#7F</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
       <c r="E24" t="s">
         <v>35</v>
       </c>
       <c r="F24" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="3"/>
+        <v>#FE</v>
+      </c>
+      <c r="I24" t="s">
+        <v>152</v>
+      </c>
+      <c r="J24" t="s">
+        <v>35</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="4"/>
+        <v>#FD</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M24" t="s">
+        <v>35</v>
+      </c>
+      <c r="N24" t="s">
+        <v>237</v>
+      </c>
+      <c r="O24" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P24" t="str">
+        <f t="shared" si="7"/>
+        <v>#BF</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
       <c r="A25" t="s">
         <v>37</v>
       </c>
       <c r="B25" t="s">
         <v>208</v>
       </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>#7F</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="1"/>
+        <v>#EF</v>
+      </c>
       <c r="E25" t="s">
         <v>236</v>
       </c>
       <c r="F25" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="G25" t="str">
+        <f t="shared" si="2"/>
+        <v>#F7</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="3"/>
+        <v>#FE</v>
+      </c>
+      <c r="I25" t="s">
+        <v>248</v>
+      </c>
+      <c r="J25" t="s">
+        <v>208</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="4"/>
+        <v>#F9</v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" si="5"/>
+        <v>#EF</v>
+      </c>
+      <c r="M25" t="s">
+        <v>236</v>
+      </c>
+      <c r="N25" t="s">
+        <v>70</v>
+      </c>
+      <c r="O25" t="str">
+        <f t="shared" si="6"/>
+        <v>#F7</v>
+      </c>
+      <c r="P25" t="str">
+        <f t="shared" si="7"/>
+        <v>#9F</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
       <c r="A26" t="s">
         <v>35</v>
       </c>
       <c r="B26" t="s">
         <v>148</v>
       </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>#FF</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="1"/>
+        <v>#CF</v>
+      </c>
       <c r="E26" t="s">
         <v>253</v>
       </c>
       <c r="F26" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="G26" t="str">
+        <f t="shared" si="2"/>
+        <v>#F3</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="3"/>
+        <v>#FF</v>
+      </c>
+      <c r="I26" t="s">
+        <v>249</v>
+      </c>
+      <c r="J26" t="s">
+        <v>148</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="4"/>
+        <v>#F1</v>
+      </c>
+      <c r="L26" t="str">
+        <f t="shared" si="5"/>
+        <v>#CF</v>
+      </c>
+      <c r="M26" t="s">
+        <v>253</v>
+      </c>
+      <c r="N26" t="s">
+        <v>251</v>
+      </c>
+      <c r="O26" t="str">
+        <f t="shared" si="6"/>
+        <v>#F3</v>
+      </c>
+      <c r="P26" t="str">
+        <f t="shared" si="7"/>
+        <v>#8F</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
       <c r="A27" t="s">
         <v>152</v>
       </c>
       <c r="B27" t="s">
         <v>251</v>
       </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>#FD</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="1"/>
+        <v>#8F</v>
+      </c>
       <c r="E27" t="s">
         <v>249</v>
       </c>
       <c r="F27" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G27" t="str">
+        <f t="shared" si="2"/>
+        <v>#F1</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="3"/>
+        <v>#BF</v>
+      </c>
+      <c r="I27" t="s">
+        <v>169</v>
+      </c>
+      <c r="J27" t="s">
+        <v>251</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="4"/>
+        <v>#60</v>
+      </c>
+      <c r="L27" t="str">
+        <f t="shared" si="5"/>
+        <v>#8F</v>
+      </c>
+      <c r="M27" t="s">
+        <v>249</v>
+      </c>
+      <c r="N27" t="s">
+        <v>156</v>
+      </c>
+      <c r="O27" t="str">
+        <f t="shared" si="6"/>
+        <v>#F1</v>
+      </c>
+      <c r="P27" t="str">
+        <f t="shared" si="7"/>
+        <v>#06</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
       <c r="A28" t="s">
         <v>248</v>
       </c>
       <c r="B28" t="s">
         <v>71</v>
       </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>#F9</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="1"/>
+        <v>#0F</v>
+      </c>
       <c r="E28" t="s">
         <v>249</v>
       </c>
       <c r="F28" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G28" t="str">
+        <f t="shared" si="2"/>
+        <v>#F1</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="3"/>
+        <v>#9F</v>
+      </c>
+      <c r="I28" t="s">
+        <v>169</v>
+      </c>
+      <c r="J28" t="s">
+        <v>71</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="4"/>
+        <v>#60</v>
+      </c>
+      <c r="L28" t="str">
+        <f t="shared" si="5"/>
+        <v>#0F</v>
+      </c>
+      <c r="M28" t="s">
+        <v>9</v>
+      </c>
+      <c r="N28" t="s">
+        <v>156</v>
+      </c>
+      <c r="O28" t="str">
+        <f t="shared" si="6"/>
+        <v>#F0</v>
+      </c>
+      <c r="P28" t="str">
+        <f t="shared" si="7"/>
+        <v>#06</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
       <c r="A29" t="s">
         <v>249</v>
       </c>
       <c r="B29" t="s">
         <v>15</v>
       </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>#F1</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="1"/>
+        <v>#07</v>
+      </c>
       <c r="E29" t="s">
         <v>33</v>
       </c>
       <c r="F29" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G29" t="str">
+        <f t="shared" si="2"/>
+        <v>#E0</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="3"/>
+        <v>#8F</v>
+      </c>
+      <c r="I29" t="s">
+        <v>39</v>
+      </c>
+      <c r="J29" t="s">
+        <v>15</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="4"/>
+        <v>#40</v>
+      </c>
+      <c r="L29" t="str">
+        <f t="shared" si="5"/>
+        <v>#07</v>
+      </c>
+      <c r="M29" t="s">
+        <v>33</v>
+      </c>
+      <c r="N29" t="s">
+        <v>21</v>
+      </c>
+      <c r="O29" t="str">
+        <f t="shared" si="6"/>
+        <v>#E0</v>
+      </c>
+      <c r="P29" t="str">
+        <f t="shared" si="7"/>
+        <v>#02</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
       <c r="A30" t="s">
         <v>169</v>
       </c>
       <c r="B30" t="s">
         <v>11</v>
       </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>#60</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="1"/>
+        <v>#03</v>
+      </c>
       <c r="E30" t="s">
         <v>76</v>
       </c>
       <c r="F30" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30" t="str">
+        <f t="shared" si="2"/>
+        <v>#C0</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="3"/>
+        <v>#06</v>
+      </c>
+      <c r="I30" t="s">
+        <v>39</v>
+      </c>
+      <c r="J30" t="s">
+        <v>11</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="4"/>
+        <v>#40</v>
+      </c>
+      <c r="L30" t="str">
+        <f t="shared" si="5"/>
+        <v>#03</v>
+      </c>
+      <c r="M30" t="s">
+        <v>76</v>
+      </c>
+      <c r="N30" t="s">
+        <v>21</v>
+      </c>
+      <c r="O30" t="str">
+        <f t="shared" si="6"/>
+        <v>#C0</v>
+      </c>
+      <c r="P30" t="str">
+        <f t="shared" si="7"/>
+        <v>#02</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
       <c r="A31" t="s">
         <v>169</v>
       </c>
       <c r="B31" t="s">
         <v>8</v>
       </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>#60</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="1"/>
+        <v>#01</v>
+      </c>
       <c r="E31" t="s">
         <v>101</v>
       </c>
       <c r="F31" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="G31" t="str">
+        <f t="shared" si="2"/>
+        <v>#80</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="3"/>
+        <v>#06</v>
+      </c>
+      <c r="I31" t="s">
+        <v>3</v>
+      </c>
+      <c r="J31" t="s">
+        <v>8</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L31" t="str">
+        <f t="shared" si="5"/>
+        <v>#01</v>
+      </c>
+      <c r="M31" t="s">
+        <v>101</v>
+      </c>
+      <c r="N31" t="s">
+        <v>3</v>
+      </c>
+      <c r="O31" t="str">
+        <f t="shared" si="6"/>
+        <v>#80</v>
+      </c>
+      <c r="P31" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
       <c r="A32" t="s">
         <v>39</v>
       </c>
       <c r="B32" t="s">
         <v>3</v>
       </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>#40</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="1"/>
+        <v>#00</v>
+      </c>
       <c r="E32" t="s">
         <v>3</v>
       </c>
       <c r="F32" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G32" t="str">
+        <f t="shared" si="2"/>
+        <v>#00</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="3"/>
+        <v>#02</v>
+      </c>
+      <c r="I32" t="s">
+        <v>3</v>
+      </c>
+      <c r="J32" t="s">
+        <v>3</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L32" t="str">
+        <f t="shared" si="5"/>
+        <v>#00</v>
+      </c>
+      <c r="M32" t="s">
+        <v>3</v>
+      </c>
+      <c r="N32" t="s">
+        <v>3</v>
+      </c>
+      <c r="O32" t="str">
+        <f t="shared" si="6"/>
+        <v>#00</v>
+      </c>
+      <c r="P32" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -10179,6 +11543,42 @@
       </c>
       <c r="F33" t="s">
         <v>21</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="2"/>
+        <v>#00</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="3"/>
+        <v>#02</v>
+      </c>
+      <c r="I33" t="s">
+        <v>3</v>
+      </c>
+      <c r="J33" t="s">
+        <v>3</v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L33" t="str">
+        <f t="shared" si="5"/>
+        <v>#00</v>
+      </c>
+      <c r="M33" t="s">
+        <v>3</v>
+      </c>
+      <c r="N33" t="s">
+        <v>3</v>
+      </c>
+      <c r="O33" t="str">
+        <f t="shared" si="6"/>
+        <v>#00</v>
+      </c>
+      <c r="P33" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fin sprite jefe fantasma
</commit_message>
<xml_diff>
--- a/doc/diseño sprites/diseno sprites.xlsx
+++ b/doc/diseño sprites/diseno sprites.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="zombi" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="fantasma" sheetId="5" r:id="rId5"/>
     <sheet name="magia" sheetId="6" r:id="rId6"/>
     <sheet name="jefevampiro" sheetId="7" r:id="rId7"/>
+    <sheet name="jefe fantaasma" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1666" uniqueCount="266">
   <si>
     <t>00011111n</t>
   </si>
@@ -792,6 +793,42 @@
   </si>
   <si>
     <t>n11110011</t>
+  </si>
+  <si>
+    <t>n00001010</t>
+  </si>
+  <si>
+    <t>n00000101</t>
+  </si>
+  <si>
+    <t>n10010111</t>
+  </si>
+  <si>
+    <t>n11100111</t>
+  </si>
+  <si>
+    <t>n10101111</t>
+  </si>
+  <si>
+    <t>n11101001</t>
+  </si>
+  <si>
+    <t>n01010011</t>
+  </si>
+  <si>
+    <t>n01100001</t>
+  </si>
+  <si>
+    <t>n01101001</t>
+  </si>
+  <si>
+    <t>n00101011</t>
+  </si>
+  <si>
+    <t>n11010110</t>
+  </si>
+  <si>
+    <t>n11010100</t>
   </si>
 </sst>
 </file>
@@ -9727,8 +9764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P17" sqref="O17:P17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -11584,4 +11621,1878 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q27" sqref="Q27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="8" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>254</v>
+      </c>
+      <c r="B1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(A1,1,1,""),2))</f>
+        <v>#0A</v>
+      </c>
+      <c r="D1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(B1,1,1,""),2))</f>
+        <v>#80</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(E1,1,1,""),2))</f>
+        <v>#01</v>
+      </c>
+      <c r="H1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(F1,1,1,""),2))</f>
+        <v>#50</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(I1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="L1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(J1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="M1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(M1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="P1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(N1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
+        <v>255</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C32" si="0">CONCATENATE("#",BIN2HEX(REPLACE(A2,1,1,""),2))</f>
+        <v>#05</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D32" si="1">CONCATENATE("#",BIN2HEX(REPLACE(B2,1,1,""),2))</f>
+        <v>#40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G33" si="2">CONCATENATE("#",BIN2HEX(REPLACE(E2,1,1,""),2))</f>
+        <v>#02</v>
+      </c>
+      <c r="H2" t="str">
+        <f t="shared" ref="H2:H33" si="3">CONCATENATE("#",BIN2HEX(REPLACE(F2,1,1,""),2))</f>
+        <v>#A0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" t="str">
+        <f t="shared" ref="K2:K33" si="4">CONCATENATE("#",BIN2HEX(REPLACE(I2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="L2" t="str">
+        <f t="shared" ref="L2:L33" si="5">CONCATENATE("#",BIN2HEX(REPLACE(J2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="M2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" t="str">
+        <f t="shared" ref="O2:O32" si="6">CONCATENATE("#",BIN2HEX(REPLACE(M2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="P2" t="str">
+        <f t="shared" ref="P2:P32" si="7">CONCATENATE("#",BIN2HEX(REPLACE(N2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>#25</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="1"/>
+        <v>#40</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>225</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="2"/>
+        <v>#02</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" si="3"/>
+        <v>#A4</v>
+      </c>
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" si="5"/>
+        <v>#00</v>
+      </c>
+      <c r="M3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3" t="str">
+        <f t="shared" si="6"/>
+        <v>#00</v>
+      </c>
+      <c r="P3" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>#1F</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v>#C0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="2"/>
+        <v>#03</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="3"/>
+        <v>#F8</v>
+      </c>
+      <c r="I4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="5"/>
+        <v>#00</v>
+      </c>
+      <c r="M4" t="s">
+        <v>3</v>
+      </c>
+      <c r="N4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O4" t="str">
+        <f t="shared" si="6"/>
+        <v>#00</v>
+      </c>
+      <c r="P4" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>#07</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v>#C0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="2"/>
+        <v>#03</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="3"/>
+        <v>#E0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="5"/>
+        <v>#00</v>
+      </c>
+      <c r="M5" t="s">
+        <v>3</v>
+      </c>
+      <c r="N5" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" t="str">
+        <f t="shared" si="6"/>
+        <v>#00</v>
+      </c>
+      <c r="P5" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>#07</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="1"/>
+        <v>#83</v>
+      </c>
+      <c r="E6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="2"/>
+        <v>#C1</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="3"/>
+        <v>#E0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="5"/>
+        <v>#03</v>
+      </c>
+      <c r="M6" t="s">
+        <v>76</v>
+      </c>
+      <c r="N6" t="s">
+        <v>3</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" si="6"/>
+        <v>#C0</v>
+      </c>
+      <c r="P6" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>#03</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="1"/>
+        <v>#1F</v>
+      </c>
+      <c r="E7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="2"/>
+        <v>#F8</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="3"/>
+        <v>#C0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" t="s">
+        <v>153</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="5"/>
+        <v>#1F</v>
+      </c>
+      <c r="M7" t="s">
+        <v>2</v>
+      </c>
+      <c r="N7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="6"/>
+        <v>#F8</v>
+      </c>
+      <c r="P7" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" t="s">
+        <v>156</v>
+      </c>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>#06</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v>#3F</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>169</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="2"/>
+        <v>#FC</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="3"/>
+        <v>#60</v>
+      </c>
+      <c r="I8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" t="s">
+        <v>43</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="5"/>
+        <v>#3F</v>
+      </c>
+      <c r="M8" t="s">
+        <v>7</v>
+      </c>
+      <c r="N8" t="s">
+        <v>3</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="6"/>
+        <v>#FC</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>#0C</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="1"/>
+        <v>#3F</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="2"/>
+        <v>#FC</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="3"/>
+        <v>#30</v>
+      </c>
+      <c r="I9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="5"/>
+        <v>#3F</v>
+      </c>
+      <c r="M9" t="s">
+        <v>7</v>
+      </c>
+      <c r="N9" t="s">
+        <v>3</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="6"/>
+        <v>#FC</v>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>#1C</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="1"/>
+        <v>#7F</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="2"/>
+        <v>#FE</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="3"/>
+        <v>#38</v>
+      </c>
+      <c r="I10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="5"/>
+        <v>#7F</v>
+      </c>
+      <c r="M10" t="s">
+        <v>14</v>
+      </c>
+      <c r="N10" t="s">
+        <v>3</v>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" si="6"/>
+        <v>#FE</v>
+      </c>
+      <c r="P10" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>#38</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
+      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="3"/>
+        <v>#1C</v>
+      </c>
+      <c r="I11" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M11" t="s">
+        <v>35</v>
+      </c>
+      <c r="N11" t="s">
+        <v>3</v>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>#3F</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
+      <c r="E12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="3"/>
+        <v>#FC</v>
+      </c>
+      <c r="I12" t="s">
+        <v>153</v>
+      </c>
+      <c r="J12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="4"/>
+        <v>#1F</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M12" t="s">
+        <v>35</v>
+      </c>
+      <c r="N12" t="s">
+        <v>2</v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" si="7"/>
+        <v>#F8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>#3F</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="3"/>
+        <v>#FC</v>
+      </c>
+      <c r="I13" t="s">
+        <v>43</v>
+      </c>
+      <c r="J13" t="s">
+        <v>35</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="4"/>
+        <v>#3F</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M13" t="s">
+        <v>35</v>
+      </c>
+      <c r="N13" t="s">
+        <v>7</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P13" t="str">
+        <f t="shared" si="7"/>
+        <v>#FC</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>#07</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
+      <c r="E14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" t="s">
+        <v>33</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="3"/>
+        <v>#E0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>102</v>
+      </c>
+      <c r="J14" t="s">
+        <v>37</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="4"/>
+        <v>#77</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="5"/>
+        <v>#7F</v>
+      </c>
+      <c r="M14" t="s">
+        <v>14</v>
+      </c>
+      <c r="N14" t="s">
+        <v>85</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="6"/>
+        <v>#FE</v>
+      </c>
+      <c r="P14" t="str">
+        <f t="shared" si="7"/>
+        <v>#EE</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>#01</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>#7F</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" t="s">
+        <v>101</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="2"/>
+        <v>#FE</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="3"/>
+        <v>#80</v>
+      </c>
+      <c r="I15" t="s">
+        <v>261</v>
+      </c>
+      <c r="J15" t="s">
+        <v>71</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="4"/>
+        <v>#61</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="5"/>
+        <v>#0F</v>
+      </c>
+      <c r="M15" t="s">
+        <v>9</v>
+      </c>
+      <c r="N15" t="s">
+        <v>158</v>
+      </c>
+      <c r="O15" t="str">
+        <f t="shared" si="6"/>
+        <v>#F0</v>
+      </c>
+      <c r="P15" t="str">
+        <f t="shared" si="7"/>
+        <v>#86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>#01</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>#0F</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" t="s">
+        <v>101</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="2"/>
+        <v>#F0</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="3"/>
+        <v>#80</v>
+      </c>
+      <c r="I16" t="s">
+        <v>261</v>
+      </c>
+      <c r="J16" t="s">
+        <v>256</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="4"/>
+        <v>#61</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="5"/>
+        <v>#97</v>
+      </c>
+      <c r="M16" t="s">
+        <v>259</v>
+      </c>
+      <c r="N16" t="s">
+        <v>158</v>
+      </c>
+      <c r="O16" t="str">
+        <f t="shared" si="6"/>
+        <v>#E9</v>
+      </c>
+      <c r="P16" t="str">
+        <f t="shared" si="7"/>
+        <v>#86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>256</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>#01</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="1"/>
+        <v>#97</v>
+      </c>
+      <c r="E18" t="s">
+        <v>259</v>
+      </c>
+      <c r="F18" t="s">
+        <v>76</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="2"/>
+        <v>#E9</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="3"/>
+        <v>#C0</v>
+      </c>
+      <c r="I18" t="s">
+        <v>262</v>
+      </c>
+      <c r="J18" t="s">
+        <v>257</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="4"/>
+        <v>#69</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="5"/>
+        <v>#E7</v>
+      </c>
+      <c r="M18" t="s">
+        <v>257</v>
+      </c>
+      <c r="N18" t="s">
+        <v>264</v>
+      </c>
+      <c r="O18" t="str">
+        <f t="shared" si="6"/>
+        <v>#E7</v>
+      </c>
+      <c r="P18" t="str">
+        <f t="shared" si="7"/>
+        <v>#D6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>257</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>#03</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="1"/>
+        <v>#E7</v>
+      </c>
+      <c r="E19" t="s">
+        <v>257</v>
+      </c>
+      <c r="F19" t="s">
+        <v>76</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="2"/>
+        <v>#E7</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="3"/>
+        <v>#C0</v>
+      </c>
+      <c r="I19" t="s">
+        <v>253</v>
+      </c>
+      <c r="J19" t="s">
+        <v>35</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="4"/>
+        <v>#F3</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M19" t="s">
+        <v>35</v>
+      </c>
+      <c r="N19" t="s">
+        <v>148</v>
+      </c>
+      <c r="O19" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P19" t="str">
+        <f t="shared" si="7"/>
+        <v>#CF</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>#03</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
+      <c r="E20" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="3"/>
+        <v>#C0</v>
+      </c>
+      <c r="I20" t="s">
+        <v>154</v>
+      </c>
+      <c r="J20" t="s">
+        <v>35</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="4"/>
+        <v>#E3</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M20" t="s">
+        <v>35</v>
+      </c>
+      <c r="N20" t="s">
+        <v>94</v>
+      </c>
+      <c r="O20" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P20" t="str">
+        <f t="shared" si="7"/>
+        <v>#C7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B21" t="s">
+        <v>206</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>#03</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="1"/>
+        <v>#DF</v>
+      </c>
+      <c r="E21" t="s">
+        <v>227</v>
+      </c>
+      <c r="F21" t="s">
+        <v>76</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="2"/>
+        <v>#FB</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="3"/>
+        <v>#C0</v>
+      </c>
+      <c r="I21" t="s">
+        <v>260</v>
+      </c>
+      <c r="J21" t="s">
+        <v>35</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="4"/>
+        <v>#53</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M21" t="s">
+        <v>35</v>
+      </c>
+      <c r="N21" t="s">
+        <v>90</v>
+      </c>
+      <c r="O21" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P21" t="str">
+        <f t="shared" si="7"/>
+        <v>#CA</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>#03</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="1"/>
+        <v>#CA</v>
+      </c>
+      <c r="E22" t="s">
+        <v>260</v>
+      </c>
+      <c r="F22" t="s">
+        <v>33</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="2"/>
+        <v>#53</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="3"/>
+        <v>#E0</v>
+      </c>
+      <c r="I22" t="s">
+        <v>263</v>
+      </c>
+      <c r="J22" t="s">
+        <v>90</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="4"/>
+        <v>#2B</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="5"/>
+        <v>#CA</v>
+      </c>
+      <c r="M22" t="s">
+        <v>260</v>
+      </c>
+      <c r="N22" t="s">
+        <v>265</v>
+      </c>
+      <c r="O22" t="str">
+        <f t="shared" si="6"/>
+        <v>#53</v>
+      </c>
+      <c r="P22" t="str">
+        <f t="shared" si="7"/>
+        <v>#D4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>#03</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="1"/>
+        <v>#E0</v>
+      </c>
+      <c r="E23" t="s">
+        <v>15</v>
+      </c>
+      <c r="F23" t="s">
+        <v>33</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="2"/>
+        <v>#07</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="3"/>
+        <v>#E0</v>
+      </c>
+      <c r="I23" t="s">
+        <v>11</v>
+      </c>
+      <c r="J23" t="s">
+        <v>33</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="4"/>
+        <v>#03</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="5"/>
+        <v>#E0</v>
+      </c>
+      <c r="M23" t="s">
+        <v>15</v>
+      </c>
+      <c r="N23" t="s">
+        <v>76</v>
+      </c>
+      <c r="O23" t="str">
+        <f t="shared" si="6"/>
+        <v>#07</v>
+      </c>
+      <c r="P23" t="str">
+        <f t="shared" si="7"/>
+        <v>#C0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" t="s">
+        <v>150</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>#03</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="1"/>
+        <v>#F5</v>
+      </c>
+      <c r="E24" t="s">
+        <v>258</v>
+      </c>
+      <c r="F24" t="s">
+        <v>76</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="2"/>
+        <v>#AF</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="3"/>
+        <v>#C0</v>
+      </c>
+      <c r="I24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" t="s">
+        <v>150</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="4"/>
+        <v>#03</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="5"/>
+        <v>#F5</v>
+      </c>
+      <c r="M24" t="s">
+        <v>258</v>
+      </c>
+      <c r="N24" t="s">
+        <v>76</v>
+      </c>
+      <c r="O24" t="str">
+        <f t="shared" si="6"/>
+        <v>#AF</v>
+      </c>
+      <c r="P24" t="str">
+        <f t="shared" si="7"/>
+        <v>#C0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>#03</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
+      <c r="E25" t="s">
+        <v>35</v>
+      </c>
+      <c r="F25" t="s">
+        <v>76</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="3"/>
+        <v>#C0</v>
+      </c>
+      <c r="I25" t="s">
+        <v>11</v>
+      </c>
+      <c r="J25" t="s">
+        <v>35</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="4"/>
+        <v>#03</v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M25" t="s">
+        <v>35</v>
+      </c>
+      <c r="N25" t="s">
+        <v>76</v>
+      </c>
+      <c r="O25" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P25" t="str">
+        <f t="shared" si="7"/>
+        <v>#C0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>#03</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
+      <c r="E26" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26" t="s">
+        <v>33</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="3"/>
+        <v>#E0</v>
+      </c>
+      <c r="I26" t="s">
+        <v>11</v>
+      </c>
+      <c r="J26" t="s">
+        <v>35</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="4"/>
+        <v>#03</v>
+      </c>
+      <c r="L26" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M26" t="s">
+        <v>35</v>
+      </c>
+      <c r="N26" t="s">
+        <v>76</v>
+      </c>
+      <c r="O26" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P26" t="str">
+        <f t="shared" si="7"/>
+        <v>#C0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>#01</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
+      <c r="E27" t="s">
+        <v>35</v>
+      </c>
+      <c r="F27" t="s">
+        <v>76</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="3"/>
+        <v>#C0</v>
+      </c>
+      <c r="I27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J27" t="s">
+        <v>35</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="4"/>
+        <v>#01</v>
+      </c>
+      <c r="L27" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M27" t="s">
+        <v>35</v>
+      </c>
+      <c r="N27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O27" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P27" t="str">
+        <f t="shared" si="7"/>
+        <v>#80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
+      <c r="E28" t="s">
+        <v>35</v>
+      </c>
+      <c r="F28" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I28" t="s">
+        <v>3</v>
+      </c>
+      <c r="J28" t="s">
+        <v>35</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L28" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M28" t="s">
+        <v>35</v>
+      </c>
+      <c r="N28" t="s">
+        <v>3</v>
+      </c>
+      <c r="O28" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P28" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
+      <c r="E29" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29" t="s">
+        <v>216</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="3"/>
+        <v>#04</v>
+      </c>
+      <c r="I29" t="s">
+        <v>3</v>
+      </c>
+      <c r="J29" t="s">
+        <v>35</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L29" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M29" t="s">
+        <v>35</v>
+      </c>
+      <c r="N29" t="s">
+        <v>3</v>
+      </c>
+      <c r="O29" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P29" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="1"/>
+        <v>#7F</v>
+      </c>
+      <c r="E30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" t="s">
+        <v>103</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="2"/>
+        <v>#FE</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="3"/>
+        <v>#08</v>
+      </c>
+      <c r="I30" t="s">
+        <v>3</v>
+      </c>
+      <c r="J30" t="s">
+        <v>37</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L30" t="str">
+        <f t="shared" si="5"/>
+        <v>#7F</v>
+      </c>
+      <c r="M30" t="s">
+        <v>14</v>
+      </c>
+      <c r="N30" t="s">
+        <v>156</v>
+      </c>
+      <c r="O30" t="str">
+        <f t="shared" si="6"/>
+        <v>#FE</v>
+      </c>
+      <c r="P30" t="str">
+        <f t="shared" si="7"/>
+        <v>#06</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="1"/>
+        <v>#3F</v>
+      </c>
+      <c r="E31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" t="s">
+        <v>105</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="2"/>
+        <v>#FC</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="3"/>
+        <v>#18</v>
+      </c>
+      <c r="I31" t="s">
+        <v>3</v>
+      </c>
+      <c r="J31" t="s">
+        <v>43</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L31" t="str">
+        <f t="shared" si="5"/>
+        <v>#3F</v>
+      </c>
+      <c r="M31" t="s">
+        <v>7</v>
+      </c>
+      <c r="N31" t="s">
+        <v>77</v>
+      </c>
+      <c r="O31" t="str">
+        <f t="shared" si="6"/>
+        <v>#FC</v>
+      </c>
+      <c r="P31" t="str">
+        <f t="shared" si="7"/>
+        <v>#1C</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" t="s">
+        <v>153</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="1"/>
+        <v>#1F</v>
+      </c>
+      <c r="E32" t="s">
+        <v>35</v>
+      </c>
+      <c r="F32" t="s">
+        <v>9</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="3"/>
+        <v>#F0</v>
+      </c>
+      <c r="I32" t="s">
+        <v>3</v>
+      </c>
+      <c r="J32" t="s">
+        <v>153</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L32" t="str">
+        <f t="shared" si="5"/>
+        <v>#1F</v>
+      </c>
+      <c r="M32" t="s">
+        <v>35</v>
+      </c>
+      <c r="N32" t="s">
+        <v>2</v>
+      </c>
+      <c r="O32" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P32" t="str">
+        <f t="shared" si="7"/>
+        <v>#F8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(A33,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="D33" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(B33,1,1,""),2))</f>
+        <v>#07</v>
+      </c>
+      <c r="E33" t="s">
+        <v>35</v>
+      </c>
+      <c r="F33" t="s">
+        <v>33</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="3"/>
+        <v>#E0</v>
+      </c>
+      <c r="I33" t="s">
+        <v>3</v>
+      </c>
+      <c r="J33" t="s">
+        <v>15</v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L33" t="str">
+        <f t="shared" si="5"/>
+        <v>#07</v>
+      </c>
+      <c r="M33" t="s">
+        <v>35</v>
+      </c>
+      <c r="N33" t="s">
+        <v>33</v>
+      </c>
+      <c r="O33" t="str">
+        <f t="shared" ref="O33" si="8">CONCATENATE("#",BIN2HEX(REPLACE(M33,1,1,""),2))</f>
+        <v>#FF</v>
+      </c>
+      <c r="P33" t="str">
+        <f t="shared" ref="P33" si="9">CONCATENATE("#",BIN2HEX(REPLACE(N33,1,1,""),2))</f>
+        <v>#E0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fin sprites mano izquierda y derecha
</commit_message>
<xml_diff>
--- a/doc/diseño sprites/diseno sprites.xlsx
+++ b/doc/diseño sprites/diseno sprites.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="2" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="3" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="zombi" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="jefe fantaasma" sheetId="8" r:id="rId8"/>
     <sheet name="jefe beholder" sheetId="9" r:id="rId9"/>
     <sheet name="jefe vampiro" sheetId="10" r:id="rId10"/>
+    <sheet name="manos" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2050" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2178" uniqueCount="298">
   <si>
     <t>00011111n</t>
   </si>
@@ -912,6 +913,21 @@
   </si>
   <si>
     <t>n10010010</t>
+  </si>
+  <si>
+    <t>n01000001</t>
+  </si>
+  <si>
+    <t>n11100001</t>
+  </si>
+  <si>
+    <t>n00110011</t>
+  </si>
+  <si>
+    <t>n00001101</t>
+  </si>
+  <si>
+    <t>n10000111</t>
   </si>
 </sst>
 </file>
@@ -3224,8 +3240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4188,6 +4204,981 @@
       <c r="H32" t="str">
         <f t="shared" si="3"/>
         <v>#3C</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(A1,1,1,""),2))</f>
+        <v>#81</v>
+      </c>
+      <c r="D1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(B1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(E1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="H1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(F1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C33" si="0">CONCATENATE("#",BIN2HEX(REPLACE(A2,1,1,""),2))</f>
+        <v>#41</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D33" si="1">CONCATENATE("#",BIN2HEX(REPLACE(B2,1,1,""),2))</f>
+        <v>#C1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G33" si="2">CONCATENATE("#",BIN2HEX(REPLACE(E2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="H2" t="str">
+        <f t="shared" ref="H2:H33" si="3">CONCATENATE("#",BIN2HEX(REPLACE(F2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>#30</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="1"/>
+        <v>#E1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="2"/>
+        <v>#00</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" t="s">
+        <v>284</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>#1C</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v>#71</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="2"/>
+        <v>#00</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" t="s">
+        <v>284</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>#0E</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v>#71</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="2"/>
+        <v>#00</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>295</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>#07</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="1"/>
+        <v>#33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="2"/>
+        <v>#07</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="3"/>
+        <v>#30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>250</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>#03</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="1"/>
+        <v>#3B</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>250</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="2"/>
+        <v>#07</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="3"/>
+        <v>#3B</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>227</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>#03</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v>#FB</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="2"/>
+        <v>#07</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="3"/>
+        <v>#FF</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>#FF</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="1"/>
+        <v>#FB</v>
+      </c>
+      <c r="E9" t="s">
+        <v>153</v>
+      </c>
+      <c r="F9" t="s">
+        <v>227</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="2"/>
+        <v>#1F</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="3"/>
+        <v>#FB</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>206</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>#7F</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="1"/>
+        <v>#DF</v>
+      </c>
+      <c r="E10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" t="s">
+        <v>206</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="2"/>
+        <v>#3F</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="3"/>
+        <v>#DF</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>237</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>#03</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v>#BF</v>
+      </c>
+      <c r="E11" t="s">
+        <v>250</v>
+      </c>
+      <c r="F11" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="2"/>
+        <v>#3B</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="3"/>
+        <v>#FF</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" t="s">
+        <v>153</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>#1F</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v>#7F</v>
+      </c>
+      <c r="E12" t="s">
+        <v>153</v>
+      </c>
+      <c r="F12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="2"/>
+        <v>#1F</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="3"/>
+        <v>#7F</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" t="s">
+        <v>215</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>#3D</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
+      <c r="E13" t="s">
+        <v>153</v>
+      </c>
+      <c r="F13" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="2"/>
+        <v>#1F</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="3"/>
+        <v>#FF</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" t="s">
+        <v>270</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>#31</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
+      <c r="E14" t="s">
+        <v>296</v>
+      </c>
+      <c r="F14" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="2"/>
+        <v>#0D</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="3"/>
+        <v>#FF</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>#20</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>#FE</v>
+      </c>
+      <c r="E15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="2"/>
+        <v>#0E</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="3"/>
+        <v>#FE</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>#20</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>#7C</v>
+      </c>
+      <c r="E16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" t="s">
+        <v>82</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="2"/>
+        <v>#00</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="3"/>
+        <v>#7C</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="1"/>
+        <v>#81</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="2"/>
+        <v>#00</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>157</v>
+      </c>
+      <c r="B19" t="s">
+        <v>159</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>#83</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="1"/>
+        <v>#82</v>
+      </c>
+      <c r="E19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="2"/>
+        <v>#00</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" t="s">
+        <v>297</v>
+      </c>
+      <c r="B20" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>#87</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="1"/>
+        <v>#0C</v>
+      </c>
+      <c r="E20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="2"/>
+        <v>#00</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>#8E</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="1"/>
+        <v>#38</v>
+      </c>
+      <c r="E21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="2"/>
+        <v>#00</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>#8E</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="1"/>
+        <v>#70</v>
+      </c>
+      <c r="E22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="2"/>
+        <v>#00</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>#CC</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="1"/>
+        <v>#E0</v>
+      </c>
+      <c r="E23" t="s">
+        <v>78</v>
+      </c>
+      <c r="F23" t="s">
+        <v>33</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="2"/>
+        <v>#0C</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="3"/>
+        <v>#E0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>#DC</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="1"/>
+        <v>#C0</v>
+      </c>
+      <c r="E24" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" t="s">
+        <v>33</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="2"/>
+        <v>#DC</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="3"/>
+        <v>#E0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>206</v>
+      </c>
+      <c r="B25" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>#DF</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="1"/>
+        <v>#C0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>35</v>
+      </c>
+      <c r="F25" t="s">
+        <v>33</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="3"/>
+        <v>#E0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>206</v>
+      </c>
+      <c r="B26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>#DF</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
+      <c r="E26" t="s">
+        <v>206</v>
+      </c>
+      <c r="F26" t="s">
+        <v>2</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="2"/>
+        <v>#DF</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="3"/>
+        <v>#F8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>227</v>
+      </c>
+      <c r="B27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>#FB</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="1"/>
+        <v>#FE</v>
+      </c>
+      <c r="E27" t="s">
+        <v>227</v>
+      </c>
+      <c r="F27" t="s">
+        <v>7</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="2"/>
+        <v>#FB</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="3"/>
+        <v>#FC</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28" t="s">
+        <v>152</v>
+      </c>
+      <c r="B28" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>#FD</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="1"/>
+        <v>#C0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>35</v>
+      </c>
+      <c r="F28" t="s">
+        <v>57</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="3"/>
+        <v>#DC</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>#FE</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="1"/>
+        <v>#F8</v>
+      </c>
+      <c r="E29" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" t="s">
+        <v>2</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="2"/>
+        <v>#FE</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="3"/>
+        <v>#F8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>#FF</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="1"/>
+        <v>#BC</v>
+      </c>
+      <c r="E30" t="s">
+        <v>35</v>
+      </c>
+      <c r="F30" t="s">
+        <v>2</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="3"/>
+        <v>#F8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" t="s">
+        <v>171</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>#FF</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="1"/>
+        <v>#8C</v>
+      </c>
+      <c r="E31" t="s">
+        <v>35</v>
+      </c>
+      <c r="F31" t="s">
+        <v>73</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="3"/>
+        <v>#B0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" t="s">
+        <v>37</v>
+      </c>
+      <c r="B32" t="s">
+        <v>216</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>#7F</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="1"/>
+        <v>#04</v>
+      </c>
+      <c r="E32" t="s">
+        <v>37</v>
+      </c>
+      <c r="F32" t="s">
+        <v>30</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="2"/>
+        <v>#7F</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="3"/>
+        <v>#70</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="A33" t="s">
+        <v>80</v>
+      </c>
+      <c r="B33" t="s">
+        <v>216</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>#3E</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="1"/>
+        <v>#04</v>
+      </c>
+      <c r="E33" t="s">
+        <v>80</v>
+      </c>
+      <c r="F33" t="s">
+        <v>3</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="2"/>
+        <v>#3E</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fin sprite jefe caballero
</commit_message>
<xml_diff>
--- a/doc/diseño sprites/diseno sprites.xlsx
+++ b/doc/diseño sprites/diseno sprites.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="3" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="6" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="zombi" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,8 @@
     <sheet name="jefe beholder" sheetId="9" r:id="rId9"/>
     <sheet name="jefe vampiro" sheetId="10" r:id="rId10"/>
     <sheet name="manos" sheetId="11" r:id="rId11"/>
+    <sheet name="jefecaballerod" sheetId="12" r:id="rId12"/>
+    <sheet name="jefecaballeroi" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2178" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2690" uniqueCount="301">
   <si>
     <t>00011111n</t>
   </si>
@@ -928,6 +930,15 @@
   </si>
   <si>
     <t>n10000111</t>
+  </si>
+  <si>
+    <t>n01110011</t>
+  </si>
+  <si>
+    <t>n01111001</t>
+  </si>
+  <si>
+    <t>n11110100</t>
   </si>
 </sst>
 </file>
@@ -4215,8 +4226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5178,6 +5189,3748 @@
       </c>
       <c r="H33" t="str">
         <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(A1,1,1,""),2))</f>
+        <v>#02</v>
+      </c>
+      <c r="D1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(B1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="E1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(E1,1,1,""),2))</f>
+        <v>#08</v>
+      </c>
+      <c r="H1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(F1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(I1,1,1,""),2))</f>
+        <v>#01</v>
+      </c>
+      <c r="L1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(J1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="M1" t="s">
+        <v>216</v>
+      </c>
+      <c r="N1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(M1,1,1,""),2))</f>
+        <v>#04</v>
+      </c>
+      <c r="P1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(N1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C33" si="0">CONCATENATE("#",BIN2HEX(REPLACE(A2,1,1,""),2))</f>
+        <v>#07</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D33" si="1">CONCATENATE("#",BIN2HEX(REPLACE(B2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="E2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G33" si="2">CONCATENATE("#",BIN2HEX(REPLACE(E2,1,1,""),2))</f>
+        <v>#08</v>
+      </c>
+      <c r="H2" t="str">
+        <f t="shared" ref="H2:H33" si="3">CONCATENATE("#",BIN2HEX(REPLACE(F2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="I2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" t="s">
+        <v>101</v>
+      </c>
+      <c r="K2" t="str">
+        <f t="shared" ref="K2:K33" si="4">CONCATENATE("#",BIN2HEX(REPLACE(I2,1,1,""),2))</f>
+        <v>#03</v>
+      </c>
+      <c r="L2" t="str">
+        <f t="shared" ref="L2:L33" si="5">CONCATENATE("#",BIN2HEX(REPLACE(J2,1,1,""),2))</f>
+        <v>#80</v>
+      </c>
+      <c r="M2" t="s">
+        <v>216</v>
+      </c>
+      <c r="N2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" t="str">
+        <f t="shared" ref="O2:O33" si="6">CONCATENATE("#",BIN2HEX(REPLACE(M2,1,1,""),2))</f>
+        <v>#04</v>
+      </c>
+      <c r="P2" t="str">
+        <f t="shared" ref="P2:P33" si="7">CONCATENATE("#",BIN2HEX(REPLACE(N2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>#07</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="1"/>
+        <v>#3F</v>
+      </c>
+      <c r="E3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="2"/>
+        <v>#0C</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" si="4"/>
+        <v>#03</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" si="5"/>
+        <v>#9F</v>
+      </c>
+      <c r="M3" t="s">
+        <v>158</v>
+      </c>
+      <c r="N3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3" t="str">
+        <f t="shared" si="6"/>
+        <v>#86</v>
+      </c>
+      <c r="P3" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>#07</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v>#7F</v>
+      </c>
+      <c r="E4" t="s">
+        <v>171</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="2"/>
+        <v>#8C</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" t="s">
+        <v>237</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="4"/>
+        <v>#03</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="5"/>
+        <v>#BF</v>
+      </c>
+      <c r="M4" t="s">
+        <v>167</v>
+      </c>
+      <c r="N4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O4" t="str">
+        <f t="shared" si="6"/>
+        <v>#C6</v>
+      </c>
+      <c r="P4" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>#07</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v>#7F</v>
+      </c>
+      <c r="E5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="2"/>
+        <v>#CC</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" t="s">
+        <v>237</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="4"/>
+        <v>#03</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="5"/>
+        <v>#BF</v>
+      </c>
+      <c r="M5" t="s">
+        <v>166</v>
+      </c>
+      <c r="N5" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" t="str">
+        <f t="shared" si="6"/>
+        <v>#E6</v>
+      </c>
+      <c r="P5" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>237</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>#07</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="1"/>
+        <v>#BF</v>
+      </c>
+      <c r="E6" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="2"/>
+        <v>#EC</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" t="s">
+        <v>206</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="4"/>
+        <v>#03</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="5"/>
+        <v>#DF</v>
+      </c>
+      <c r="M6" t="s">
+        <v>164</v>
+      </c>
+      <c r="N6" t="s">
+        <v>3</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" si="6"/>
+        <v>#F6</v>
+      </c>
+      <c r="P6" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>206</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>#03</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="1"/>
+        <v>#DF</v>
+      </c>
+      <c r="E7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="2"/>
+        <v>#CC</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" t="s">
+        <v>208</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="4"/>
+        <v>#01</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="5"/>
+        <v>#EF</v>
+      </c>
+      <c r="M7" t="s">
+        <v>166</v>
+      </c>
+      <c r="N7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="6"/>
+        <v>#E6</v>
+      </c>
+      <c r="P7" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>206</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>#03</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v>#DF</v>
+      </c>
+      <c r="E8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="2"/>
+        <v>#F0</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" t="s">
+        <v>208</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="4"/>
+        <v>#01</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="5"/>
+        <v>#EF</v>
+      </c>
+      <c r="M8" t="s">
+        <v>2</v>
+      </c>
+      <c r="N8" t="s">
+        <v>3</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="6"/>
+        <v>#F8</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>#02</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="1"/>
+        <v>#70</v>
+      </c>
+      <c r="E9" t="s">
+        <v>234</v>
+      </c>
+      <c r="F9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="2"/>
+        <v>#10</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" t="s">
+        <v>79</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="4"/>
+        <v>#01</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="5"/>
+        <v>#38</v>
+      </c>
+      <c r="M9" t="s">
+        <v>103</v>
+      </c>
+      <c r="N9" t="s">
+        <v>3</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="6"/>
+        <v>#08</v>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>#03</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="1"/>
+        <v>#F8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="2"/>
+        <v>#20</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I10" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="4"/>
+        <v>#01</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="5"/>
+        <v>#FC</v>
+      </c>
+      <c r="M10" t="s">
+        <v>234</v>
+      </c>
+      <c r="N10" t="s">
+        <v>3</v>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" si="6"/>
+        <v>#10</v>
+      </c>
+      <c r="P10" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>#03</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v>#FE</v>
+      </c>
+      <c r="E11" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="2"/>
+        <v>#E0</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I11" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M11" t="s">
+        <v>30</v>
+      </c>
+      <c r="N11" t="s">
+        <v>3</v>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" si="6"/>
+        <v>#70</v>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>#01</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v>#FE</v>
+      </c>
+      <c r="E12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="2"/>
+        <v>#E0</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I12" t="s">
+        <v>3</v>
+      </c>
+      <c r="J12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M12" t="s">
+        <v>30</v>
+      </c>
+      <c r="N12" t="s">
+        <v>3</v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" si="6"/>
+        <v>#70</v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>#07</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v>#FE</v>
+      </c>
+      <c r="E13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="2"/>
+        <v>#F8</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I13" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="4"/>
+        <v>#07</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="5"/>
+        <v>#FE</v>
+      </c>
+      <c r="M13" t="s">
+        <v>2</v>
+      </c>
+      <c r="N13" t="s">
+        <v>3</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" si="6"/>
+        <v>#F8</v>
+      </c>
+      <c r="P13" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" t="s">
+        <v>237</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>#0F</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>#BF</v>
+      </c>
+      <c r="E14" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="2"/>
+        <v>#FC</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I14" t="s">
+        <v>71</v>
+      </c>
+      <c r="J14" t="s">
+        <v>237</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="4"/>
+        <v>#0F</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="5"/>
+        <v>#BF</v>
+      </c>
+      <c r="M14" t="s">
+        <v>7</v>
+      </c>
+      <c r="N14" t="s">
+        <v>3</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="6"/>
+        <v>#FC</v>
+      </c>
+      <c r="P14" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>#0F</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>#9F</v>
+      </c>
+      <c r="E15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="2"/>
+        <v>#FE</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I15" t="s">
+        <v>71</v>
+      </c>
+      <c r="J15" t="s">
+        <v>70</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="4"/>
+        <v>#0F</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="5"/>
+        <v>#9F</v>
+      </c>
+      <c r="M15" t="s">
+        <v>14</v>
+      </c>
+      <c r="N15" t="s">
+        <v>3</v>
+      </c>
+      <c r="O15" t="str">
+        <f t="shared" si="6"/>
+        <v>#FE</v>
+      </c>
+      <c r="P15" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" t="s">
+        <v>153</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>#1F</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
+      <c r="E16" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="2"/>
+        <v>#FE</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I16" t="s">
+        <v>153</v>
+      </c>
+      <c r="J16" t="s">
+        <v>35</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="4"/>
+        <v>#1F</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M16" t="s">
+        <v>14</v>
+      </c>
+      <c r="N16" t="s">
+        <v>3</v>
+      </c>
+      <c r="O16" t="str">
+        <f t="shared" si="6"/>
+        <v>#FE</v>
+      </c>
+      <c r="P16" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" t="s">
+        <v>153</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>#1F</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
+      <c r="E18" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="2"/>
+        <v>#DC</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I18" t="s">
+        <v>153</v>
+      </c>
+      <c r="J18" t="s">
+        <v>35</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="4"/>
+        <v>#1F</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M18" t="s">
+        <v>57</v>
+      </c>
+      <c r="N18" t="s">
+        <v>3</v>
+      </c>
+      <c r="O18" t="str">
+        <f t="shared" si="6"/>
+        <v>#DC</v>
+      </c>
+      <c r="P18" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19" t="s">
+        <v>147</v>
+      </c>
+      <c r="B19" t="s">
+        <v>221</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>#1E</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="1"/>
+        <v>#5F</v>
+      </c>
+      <c r="E19" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="2"/>
+        <v>#DC</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I19" t="s">
+        <v>23</v>
+      </c>
+      <c r="J19" t="s">
+        <v>221</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="4"/>
+        <v>#3C</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="5"/>
+        <v>#5F</v>
+      </c>
+      <c r="M19" t="s">
+        <v>57</v>
+      </c>
+      <c r="N19" t="s">
+        <v>3</v>
+      </c>
+      <c r="O19" t="str">
+        <f t="shared" si="6"/>
+        <v>#DC</v>
+      </c>
+      <c r="P19" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>206</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>#3C</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="1"/>
+        <v>#DF</v>
+      </c>
+      <c r="E20" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="2"/>
+        <v>#DC</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I20" t="s">
+        <v>35</v>
+      </c>
+      <c r="J20" t="s">
+        <v>206</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="4"/>
+        <v>#FF</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="5"/>
+        <v>#DF</v>
+      </c>
+      <c r="M20" t="s">
+        <v>57</v>
+      </c>
+      <c r="N20" t="s">
+        <v>3</v>
+      </c>
+      <c r="O20" t="str">
+        <f t="shared" si="6"/>
+        <v>#DC</v>
+      </c>
+      <c r="P20" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B21" t="s">
+        <v>206</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>#FF</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="1"/>
+        <v>#DF</v>
+      </c>
+      <c r="E21" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="2"/>
+        <v>#DC</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I21" t="s">
+        <v>257</v>
+      </c>
+      <c r="J21" t="s">
+        <v>206</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="4"/>
+        <v>#E7</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="5"/>
+        <v>#DF</v>
+      </c>
+      <c r="M21" t="s">
+        <v>207</v>
+      </c>
+      <c r="N21" t="s">
+        <v>3</v>
+      </c>
+      <c r="O21" t="str">
+        <f t="shared" si="6"/>
+        <v>#DE</v>
+      </c>
+      <c r="P21" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" t="s">
+        <v>257</v>
+      </c>
+      <c r="B22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>#E7</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="1"/>
+        <v>#5F</v>
+      </c>
+      <c r="E22" t="s">
+        <v>170</v>
+      </c>
+      <c r="F22" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="2"/>
+        <v>#9E</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I22" t="s">
+        <v>41</v>
+      </c>
+      <c r="J22" t="s">
+        <v>221</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="4"/>
+        <v>#81</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="5"/>
+        <v>#5F</v>
+      </c>
+      <c r="M22" t="s">
+        <v>237</v>
+      </c>
+      <c r="N22" t="s">
+        <v>14</v>
+      </c>
+      <c r="O22" t="str">
+        <f t="shared" si="6"/>
+        <v>#BF</v>
+      </c>
+      <c r="P22" t="str">
+        <f t="shared" si="7"/>
+        <v>#FE</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>#81</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="1"/>
+        <v>#2F</v>
+      </c>
+      <c r="E23" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="2"/>
+        <v>#7F</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="3"/>
+        <v>#FE</v>
+      </c>
+      <c r="I23" t="s">
+        <v>41</v>
+      </c>
+      <c r="J23" t="s">
+        <v>89</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="4"/>
+        <v>#81</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="5"/>
+        <v>#2F</v>
+      </c>
+      <c r="M23" t="s">
+        <v>37</v>
+      </c>
+      <c r="N23" t="s">
+        <v>35</v>
+      </c>
+      <c r="O23" t="str">
+        <f t="shared" si="6"/>
+        <v>#7F</v>
+      </c>
+      <c r="P23" t="str">
+        <f t="shared" si="7"/>
+        <v>#FF</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>#81</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="1"/>
+        <v>#7F</v>
+      </c>
+      <c r="E24" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" t="s">
+        <v>35</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="3"/>
+        <v>#FF</v>
+      </c>
+      <c r="I24" t="s">
+        <v>257</v>
+      </c>
+      <c r="J24" t="s">
+        <v>37</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="4"/>
+        <v>#E7</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="5"/>
+        <v>#7F</v>
+      </c>
+      <c r="M24" t="s">
+        <v>148</v>
+      </c>
+      <c r="N24" t="s">
+        <v>35</v>
+      </c>
+      <c r="O24" t="str">
+        <f t="shared" si="6"/>
+        <v>#CF</v>
+      </c>
+      <c r="P24" t="str">
+        <f t="shared" si="7"/>
+        <v>#FF</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" t="s">
+        <v>257</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>#E7</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="1"/>
+        <v>#7F</v>
+      </c>
+      <c r="E25" t="s">
+        <v>148</v>
+      </c>
+      <c r="F25" t="s">
+        <v>35</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="2"/>
+        <v>#CF</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="3"/>
+        <v>#FF</v>
+      </c>
+      <c r="I25" t="s">
+        <v>257</v>
+      </c>
+      <c r="J25" t="s">
+        <v>37</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="4"/>
+        <v>#E7</v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" si="5"/>
+        <v>#7F</v>
+      </c>
+      <c r="M25" t="s">
+        <v>148</v>
+      </c>
+      <c r="N25" t="s">
+        <v>14</v>
+      </c>
+      <c r="O25" t="str">
+        <f t="shared" si="6"/>
+        <v>#CF</v>
+      </c>
+      <c r="P25" t="str">
+        <f t="shared" si="7"/>
+        <v>#FE</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" t="s">
+        <v>257</v>
+      </c>
+      <c r="B26" t="s">
+        <v>204</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>#E7</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="1"/>
+        <v>#7B</v>
+      </c>
+      <c r="E26" t="s">
+        <v>148</v>
+      </c>
+      <c r="F26" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="2"/>
+        <v>#CF</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="3"/>
+        <v>#FE</v>
+      </c>
+      <c r="I26" t="s">
+        <v>161</v>
+      </c>
+      <c r="J26" t="s">
+        <v>37</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="4"/>
+        <v>#67</v>
+      </c>
+      <c r="L26" t="str">
+        <f t="shared" si="5"/>
+        <v>#7F</v>
+      </c>
+      <c r="M26" t="s">
+        <v>67</v>
+      </c>
+      <c r="N26" t="s">
+        <v>3</v>
+      </c>
+      <c r="O26" t="str">
+        <f t="shared" si="6"/>
+        <v>#CC</v>
+      </c>
+      <c r="P26" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" t="s">
+        <v>161</v>
+      </c>
+      <c r="B27" t="s">
+        <v>204</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>#67</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="1"/>
+        <v>#7B</v>
+      </c>
+      <c r="E27" t="s">
+        <v>171</v>
+      </c>
+      <c r="F27" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="2"/>
+        <v>#8C</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I27" t="s">
+        <v>80</v>
+      </c>
+      <c r="J27" t="s">
+        <v>37</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="4"/>
+        <v>#3E</v>
+      </c>
+      <c r="L27" t="str">
+        <f t="shared" si="5"/>
+        <v>#7F</v>
+      </c>
+      <c r="M27" t="s">
+        <v>172</v>
+      </c>
+      <c r="N27" t="s">
+        <v>3</v>
+      </c>
+      <c r="O27" t="str">
+        <f t="shared" si="6"/>
+        <v>#84</v>
+      </c>
+      <c r="P27" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" t="s">
+        <v>227</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>#3E</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="1"/>
+        <v>#FB</v>
+      </c>
+      <c r="E28" t="s">
+        <v>223</v>
+      </c>
+      <c r="F28" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="2"/>
+        <v>#C4</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I28" t="s">
+        <v>77</v>
+      </c>
+      <c r="J28" t="s">
+        <v>37</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="4"/>
+        <v>#1C</v>
+      </c>
+      <c r="L28" t="str">
+        <f t="shared" si="5"/>
+        <v>#7F</v>
+      </c>
+      <c r="M28" t="s">
+        <v>101</v>
+      </c>
+      <c r="N28" t="s">
+        <v>3</v>
+      </c>
+      <c r="O28" t="str">
+        <f t="shared" si="6"/>
+        <v>#80</v>
+      </c>
+      <c r="P28" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" t="s">
+        <v>227</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>#1C</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="1"/>
+        <v>#FB</v>
+      </c>
+      <c r="E29" t="s">
+        <v>76</v>
+      </c>
+      <c r="F29" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="2"/>
+        <v>#C0</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I29" t="s">
+        <v>3</v>
+      </c>
+      <c r="J29" t="s">
+        <v>204</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L29" t="str">
+        <f t="shared" si="5"/>
+        <v>#7B</v>
+      </c>
+      <c r="M29" t="s">
+        <v>101</v>
+      </c>
+      <c r="N29" t="s">
+        <v>3</v>
+      </c>
+      <c r="O29" t="str">
+        <f t="shared" si="6"/>
+        <v>#80</v>
+      </c>
+      <c r="P29" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
+        <v>227</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="1"/>
+        <v>#FB</v>
+      </c>
+      <c r="E30" t="s">
+        <v>33</v>
+      </c>
+      <c r="F30" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="2"/>
+        <v>#E0</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I30" t="s">
+        <v>3</v>
+      </c>
+      <c r="J30" t="s">
+        <v>298</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L30" t="str">
+        <f t="shared" si="5"/>
+        <v>#73</v>
+      </c>
+      <c r="M30" t="s">
+        <v>101</v>
+      </c>
+      <c r="N30" t="s">
+        <v>3</v>
+      </c>
+      <c r="O30" t="str">
+        <f t="shared" si="6"/>
+        <v>#80</v>
+      </c>
+      <c r="P30" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" t="s">
+        <v>284</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="1"/>
+        <v>#71</v>
+      </c>
+      <c r="E31" t="s">
+        <v>33</v>
+      </c>
+      <c r="F31" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="2"/>
+        <v>#E0</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I31" t="s">
+        <v>3</v>
+      </c>
+      <c r="J31" t="s">
+        <v>298</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L31" t="str">
+        <f t="shared" si="5"/>
+        <v>#73</v>
+      </c>
+      <c r="M31" t="s">
+        <v>101</v>
+      </c>
+      <c r="N31" t="s">
+        <v>3</v>
+      </c>
+      <c r="O31" t="str">
+        <f t="shared" si="6"/>
+        <v>#80</v>
+      </c>
+      <c r="P31" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" t="s">
+        <v>249</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="1"/>
+        <v>#F1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" t="s">
+        <v>3</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="2"/>
+        <v>#F0</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I32" t="s">
+        <v>3</v>
+      </c>
+      <c r="J32" t="s">
+        <v>204</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L32" t="str">
+        <f t="shared" si="5"/>
+        <v>#7B</v>
+      </c>
+      <c r="M32" t="s">
+        <v>76</v>
+      </c>
+      <c r="N32" t="s">
+        <v>3</v>
+      </c>
+      <c r="O32" t="str">
+        <f t="shared" si="6"/>
+        <v>#C0</v>
+      </c>
+      <c r="P32" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="1"/>
+        <v>#F8</v>
+      </c>
+      <c r="E33" t="s">
+        <v>2</v>
+      </c>
+      <c r="F33" t="s">
+        <v>3</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="2"/>
+        <v>#F8</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I33" t="s">
+        <v>3</v>
+      </c>
+      <c r="J33" t="s">
+        <v>37</v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L33" t="str">
+        <f t="shared" si="5"/>
+        <v>#7F</v>
+      </c>
+      <c r="M33" t="s">
+        <v>9</v>
+      </c>
+      <c r="N33" t="s">
+        <v>3</v>
+      </c>
+      <c r="O33" t="str">
+        <f t="shared" si="6"/>
+        <v>#F0</v>
+      </c>
+      <c r="P33" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(A1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="D1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(B1,1,1,""),2))</f>
+        <v>#10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(E1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="H1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(F1,1,1,""),2))</f>
+        <v>#40</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(I1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="L1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(J1,1,1,""),2))</f>
+        <v>#20</v>
+      </c>
+      <c r="M1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" t="s">
+        <v>101</v>
+      </c>
+      <c r="O1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(M1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="P1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(N1,1,1,""),2))</f>
+        <v>#80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C33" si="0">CONCATENATE("#",BIN2HEX(REPLACE(A2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D33" si="1">CONCATENATE("#",BIN2HEX(REPLACE(B2,1,1,""),2))</f>
+        <v>#10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G33" si="2">CONCATENATE("#",BIN2HEX(REPLACE(E2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="H2" t="str">
+        <f t="shared" ref="H2:H33" si="3">CONCATENATE("#",BIN2HEX(REPLACE(F2,1,1,""),2))</f>
+        <v>#E0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K2" t="str">
+        <f t="shared" ref="K2:K33" si="4">CONCATENATE("#",BIN2HEX(REPLACE(I2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="L2" t="str">
+        <f t="shared" ref="L2:L33" si="5">CONCATENATE("#",BIN2HEX(REPLACE(J2,1,1,""),2))</f>
+        <v>#20</v>
+      </c>
+      <c r="M2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" t="s">
+        <v>76</v>
+      </c>
+      <c r="O2" t="str">
+        <f t="shared" ref="O2:O32" si="6">CONCATENATE("#",BIN2HEX(REPLACE(M2,1,1,""),2))</f>
+        <v>#01</v>
+      </c>
+      <c r="P2" t="str">
+        <f t="shared" ref="P2:P32" si="7">CONCATENATE("#",BIN2HEX(REPLACE(N2,1,1,""),2))</f>
+        <v>#C0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="1"/>
+        <v>#30</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="2"/>
+        <v>#FC</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" si="3"/>
+        <v>#E0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>261</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" si="5"/>
+        <v>#61</v>
+      </c>
+      <c r="M3" t="s">
+        <v>248</v>
+      </c>
+      <c r="N3" t="s">
+        <v>76</v>
+      </c>
+      <c r="O3" t="str">
+        <f t="shared" si="6"/>
+        <v>#F9</v>
+      </c>
+      <c r="P3" t="str">
+        <f t="shared" si="7"/>
+        <v>#C0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>270</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v>#31</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="2"/>
+        <v>#FE</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="3"/>
+        <v>#E0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>155</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="5"/>
+        <v>#63</v>
+      </c>
+      <c r="M4" t="s">
+        <v>152</v>
+      </c>
+      <c r="N4" t="s">
+        <v>76</v>
+      </c>
+      <c r="O4" t="str">
+        <f t="shared" si="6"/>
+        <v>#FD</v>
+      </c>
+      <c r="P4" t="str">
+        <f t="shared" si="7"/>
+        <v>#C0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>295</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v>#33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="2"/>
+        <v>#FE</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="3"/>
+        <v>#E0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" t="s">
+        <v>161</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="5"/>
+        <v>#67</v>
+      </c>
+      <c r="M5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" t="s">
+        <v>76</v>
+      </c>
+      <c r="O5" t="str">
+        <f t="shared" si="6"/>
+        <v>#02</v>
+      </c>
+      <c r="P5" t="str">
+        <f t="shared" si="7"/>
+        <v>#C0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="1"/>
+        <v>#37</v>
+      </c>
+      <c r="E6" t="s">
+        <v>152</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="2"/>
+        <v>#FD</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="3"/>
+        <v>#E0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" t="s">
+        <v>202</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="5"/>
+        <v>#6F</v>
+      </c>
+      <c r="M6" t="s">
+        <v>227</v>
+      </c>
+      <c r="N6" t="s">
+        <v>76</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" si="6"/>
+        <v>#FB</v>
+      </c>
+      <c r="P6" t="str">
+        <f t="shared" si="7"/>
+        <v>#C0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>295</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="1"/>
+        <v>#33</v>
+      </c>
+      <c r="E7" t="s">
+        <v>227</v>
+      </c>
+      <c r="F7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="2"/>
+        <v>#FB</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="3"/>
+        <v>#C0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" t="s">
+        <v>161</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="5"/>
+        <v>#67</v>
+      </c>
+      <c r="M7" t="s">
+        <v>236</v>
+      </c>
+      <c r="N7" t="s">
+        <v>101</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="6"/>
+        <v>#F7</v>
+      </c>
+      <c r="P7" t="str">
+        <f t="shared" si="7"/>
+        <v>#80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v>#0F</v>
+      </c>
+      <c r="E8" t="s">
+        <v>227</v>
+      </c>
+      <c r="F8" t="s">
+        <v>76</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="2"/>
+        <v>#FB</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="3"/>
+        <v>#C0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" t="s">
+        <v>153</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="5"/>
+        <v>#1F</v>
+      </c>
+      <c r="M8" t="s">
+        <v>236</v>
+      </c>
+      <c r="N8" t="s">
+        <v>101</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="6"/>
+        <v>#F7</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" si="7"/>
+        <v>#80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>103</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="1"/>
+        <v>#08</v>
+      </c>
+      <c r="E9" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="2"/>
+        <v>#0E</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="3"/>
+        <v>#40</v>
+      </c>
+      <c r="I9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" t="s">
+        <v>234</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="5"/>
+        <v>#10</v>
+      </c>
+      <c r="M9" t="s">
+        <v>77</v>
+      </c>
+      <c r="N9" t="s">
+        <v>101</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="6"/>
+        <v>#1C</v>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" si="7"/>
+        <v>#80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>216</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="1"/>
+        <v>#04</v>
+      </c>
+      <c r="E10" t="s">
+        <v>153</v>
+      </c>
+      <c r="F10" t="s">
+        <v>76</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="2"/>
+        <v>#1F</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="3"/>
+        <v>#C0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" t="s">
+        <v>103</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="5"/>
+        <v>#08</v>
+      </c>
+      <c r="M10" t="s">
+        <v>43</v>
+      </c>
+      <c r="N10" t="s">
+        <v>101</v>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" si="6"/>
+        <v>#3F</v>
+      </c>
+      <c r="P10" t="str">
+        <f t="shared" si="7"/>
+        <v>#80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v>#07</v>
+      </c>
+      <c r="E11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="2"/>
+        <v>#7F</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="3"/>
+        <v>#C0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" t="s">
+        <v>65</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="5"/>
+        <v>#0E</v>
+      </c>
+      <c r="M11" t="s">
+        <v>35</v>
+      </c>
+      <c r="N11" t="s">
+        <v>3</v>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v>#07</v>
+      </c>
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" t="s">
+        <v>101</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="2"/>
+        <v>#7F</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="3"/>
+        <v>#80</v>
+      </c>
+      <c r="I12" t="s">
+        <v>3</v>
+      </c>
+      <c r="J12" t="s">
+        <v>65</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="5"/>
+        <v>#0E</v>
+      </c>
+      <c r="M12" t="s">
+        <v>35</v>
+      </c>
+      <c r="N12" t="s">
+        <v>3</v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>153</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v>#1F</v>
+      </c>
+      <c r="E13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="2"/>
+        <v>#7F</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="3"/>
+        <v>#E0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>3</v>
+      </c>
+      <c r="J13" t="s">
+        <v>153</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="5"/>
+        <v>#1F</v>
+      </c>
+      <c r="M13" t="s">
+        <v>37</v>
+      </c>
+      <c r="N13" t="s">
+        <v>33</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" si="6"/>
+        <v>#7F</v>
+      </c>
+      <c r="P13" t="str">
+        <f t="shared" si="7"/>
+        <v>#E0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>#3F</v>
+      </c>
+      <c r="E14" t="s">
+        <v>152</v>
+      </c>
+      <c r="F14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="2"/>
+        <v>#FD</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="3"/>
+        <v>#F0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>3</v>
+      </c>
+      <c r="J14" t="s">
+        <v>43</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="5"/>
+        <v>#3F</v>
+      </c>
+      <c r="M14" t="s">
+        <v>152</v>
+      </c>
+      <c r="N14" t="s">
+        <v>9</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="6"/>
+        <v>#FD</v>
+      </c>
+      <c r="P14" t="str">
+        <f t="shared" si="7"/>
+        <v>#F0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>#7F</v>
+      </c>
+      <c r="E15" t="s">
+        <v>248</v>
+      </c>
+      <c r="F15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="2"/>
+        <v>#F9</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="3"/>
+        <v>#F0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>3</v>
+      </c>
+      <c r="J15" t="s">
+        <v>37</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="5"/>
+        <v>#7F</v>
+      </c>
+      <c r="M15" t="s">
+        <v>248</v>
+      </c>
+      <c r="N15" t="s">
+        <v>9</v>
+      </c>
+      <c r="O15" t="str">
+        <f t="shared" si="6"/>
+        <v>#F9</v>
+      </c>
+      <c r="P15" t="str">
+        <f t="shared" si="7"/>
+        <v>#F0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>#7F</v>
+      </c>
+      <c r="E16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="3"/>
+        <v>#F8</v>
+      </c>
+      <c r="I16" t="s">
+        <v>3</v>
+      </c>
+      <c r="J16" t="s">
+        <v>37</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="5"/>
+        <v>#7F</v>
+      </c>
+      <c r="M16" t="s">
+        <v>35</v>
+      </c>
+      <c r="N16" t="s">
+        <v>2</v>
+      </c>
+      <c r="O16" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P16" t="str">
+        <f t="shared" si="7"/>
+        <v>#F8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>250</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="1"/>
+        <v>#3B</v>
+      </c>
+      <c r="E18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="3"/>
+        <v>#F8</v>
+      </c>
+      <c r="I18" t="s">
+        <v>3</v>
+      </c>
+      <c r="J18" t="s">
+        <v>250</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="5"/>
+        <v>#3B</v>
+      </c>
+      <c r="M18" t="s">
+        <v>14</v>
+      </c>
+      <c r="N18" t="s">
+        <v>2</v>
+      </c>
+      <c r="O18" t="str">
+        <f t="shared" si="6"/>
+        <v>#FE</v>
+      </c>
+      <c r="P18" t="str">
+        <f t="shared" si="7"/>
+        <v>#F8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>250</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="1"/>
+        <v>#3B</v>
+      </c>
+      <c r="E19" t="s">
+        <v>212</v>
+      </c>
+      <c r="F19" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="2"/>
+        <v>#FA</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="3"/>
+        <v>#78</v>
+      </c>
+      <c r="I19" t="s">
+        <v>3</v>
+      </c>
+      <c r="J19" t="s">
+        <v>250</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="5"/>
+        <v>#3B</v>
+      </c>
+      <c r="M19" t="s">
+        <v>212</v>
+      </c>
+      <c r="N19" t="s">
+        <v>23</v>
+      </c>
+      <c r="O19" t="str">
+        <f t="shared" si="6"/>
+        <v>#FA</v>
+      </c>
+      <c r="P19" t="str">
+        <f t="shared" si="7"/>
+        <v>#3C</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>250</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="1"/>
+        <v>#3B</v>
+      </c>
+      <c r="E20" t="s">
+        <v>227</v>
+      </c>
+      <c r="F20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="2"/>
+        <v>#FB</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="3"/>
+        <v>#3C</v>
+      </c>
+      <c r="I20" t="s">
+        <v>3</v>
+      </c>
+      <c r="J20" t="s">
+        <v>250</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="5"/>
+        <v>#3B</v>
+      </c>
+      <c r="M20" t="s">
+        <v>227</v>
+      </c>
+      <c r="N20" t="s">
+        <v>35</v>
+      </c>
+      <c r="O20" t="str">
+        <f t="shared" si="6"/>
+        <v>#FB</v>
+      </c>
+      <c r="P20" t="str">
+        <f t="shared" si="7"/>
+        <v>#FF</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>250</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="1"/>
+        <v>#3B</v>
+      </c>
+      <c r="E21" t="s">
+        <v>227</v>
+      </c>
+      <c r="F21" t="s">
+        <v>35</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="2"/>
+        <v>#FB</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="3"/>
+        <v>#FF</v>
+      </c>
+      <c r="I21" t="s">
+        <v>3</v>
+      </c>
+      <c r="J21" t="s">
+        <v>204</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="5"/>
+        <v>#7B</v>
+      </c>
+      <c r="M21" t="s">
+        <v>227</v>
+      </c>
+      <c r="N21" t="s">
+        <v>257</v>
+      </c>
+      <c r="O21" t="str">
+        <f t="shared" si="6"/>
+        <v>#FB</v>
+      </c>
+      <c r="P21" t="str">
+        <f t="shared" si="7"/>
+        <v>#E7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" t="s">
+        <v>299</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="1"/>
+        <v>#79</v>
+      </c>
+      <c r="E22" t="s">
+        <v>212</v>
+      </c>
+      <c r="F22" t="s">
+        <v>257</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="2"/>
+        <v>#FA</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="3"/>
+        <v>#E7</v>
+      </c>
+      <c r="I22" t="s">
+        <v>37</v>
+      </c>
+      <c r="J22" t="s">
+        <v>152</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="4"/>
+        <v>#7F</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="5"/>
+        <v>#FD</v>
+      </c>
+      <c r="M22" t="s">
+        <v>212</v>
+      </c>
+      <c r="N22" t="s">
+        <v>41</v>
+      </c>
+      <c r="O22" t="str">
+        <f t="shared" si="6"/>
+        <v>#FA</v>
+      </c>
+      <c r="P22" t="str">
+        <f t="shared" si="7"/>
+        <v>#81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>#7F</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="1"/>
+        <v>#FE</v>
+      </c>
+      <c r="E23" t="s">
+        <v>300</v>
+      </c>
+      <c r="F23" t="s">
+        <v>41</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="2"/>
+        <v>#F4</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="3"/>
+        <v>#81</v>
+      </c>
+      <c r="I23" t="s">
+        <v>35</v>
+      </c>
+      <c r="J23" t="s">
+        <v>14</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="4"/>
+        <v>#FF</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="5"/>
+        <v>#FE</v>
+      </c>
+      <c r="M23" t="s">
+        <v>300</v>
+      </c>
+      <c r="N23" t="s">
+        <v>41</v>
+      </c>
+      <c r="O23" t="str">
+        <f t="shared" si="6"/>
+        <v>#F4</v>
+      </c>
+      <c r="P23" t="str">
+        <f t="shared" si="7"/>
+        <v>#81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>#FF</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
+      <c r="E24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" t="s">
+        <v>41</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="2"/>
+        <v>#FE</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="3"/>
+        <v>#81</v>
+      </c>
+      <c r="I24" t="s">
+        <v>35</v>
+      </c>
+      <c r="J24" t="s">
+        <v>253</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="4"/>
+        <v>#FF</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="5"/>
+        <v>#F3</v>
+      </c>
+      <c r="M24" t="s">
+        <v>14</v>
+      </c>
+      <c r="N24" t="s">
+        <v>257</v>
+      </c>
+      <c r="O24" t="str">
+        <f t="shared" si="6"/>
+        <v>#FE</v>
+      </c>
+      <c r="P24" t="str">
+        <f t="shared" si="7"/>
+        <v>#E7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" t="s">
+        <v>253</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>#FF</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="1"/>
+        <v>#F3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" t="s">
+        <v>257</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="2"/>
+        <v>#FE</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="3"/>
+        <v>#E7</v>
+      </c>
+      <c r="I25" t="s">
+        <v>37</v>
+      </c>
+      <c r="J25" t="s">
+        <v>253</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="4"/>
+        <v>#7F</v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" si="5"/>
+        <v>#F3</v>
+      </c>
+      <c r="M25" t="s">
+        <v>14</v>
+      </c>
+      <c r="N25" t="s">
+        <v>257</v>
+      </c>
+      <c r="O25" t="str">
+        <f t="shared" si="6"/>
+        <v>#FE</v>
+      </c>
+      <c r="P25" t="str">
+        <f t="shared" si="7"/>
+        <v>#E7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" t="s">
+        <v>253</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>#7F</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="1"/>
+        <v>#F3</v>
+      </c>
+      <c r="E26" t="s">
+        <v>207</v>
+      </c>
+      <c r="F26" t="s">
+        <v>257</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="2"/>
+        <v>#DE</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="3"/>
+        <v>#E7</v>
+      </c>
+      <c r="I26" t="s">
+        <v>3</v>
+      </c>
+      <c r="J26" t="s">
+        <v>295</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L26" t="str">
+        <f t="shared" si="5"/>
+        <v>#33</v>
+      </c>
+      <c r="M26" t="s">
+        <v>14</v>
+      </c>
+      <c r="N26" t="s">
+        <v>166</v>
+      </c>
+      <c r="O26" t="str">
+        <f t="shared" si="6"/>
+        <v>#FE</v>
+      </c>
+      <c r="P26" t="str">
+        <f t="shared" si="7"/>
+        <v>#E6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
+        <v>270</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="1"/>
+        <v>#31</v>
+      </c>
+      <c r="E27" t="s">
+        <v>207</v>
+      </c>
+      <c r="F27" t="s">
+        <v>166</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="2"/>
+        <v>#DE</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="3"/>
+        <v>#E6</v>
+      </c>
+      <c r="I27" t="s">
+        <v>3</v>
+      </c>
+      <c r="J27" t="s">
+        <v>50</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L27" t="str">
+        <f t="shared" si="5"/>
+        <v>#21</v>
+      </c>
+      <c r="M27" t="s">
+        <v>14</v>
+      </c>
+      <c r="N27" t="s">
+        <v>82</v>
+      </c>
+      <c r="O27" t="str">
+        <f t="shared" si="6"/>
+        <v>#FE</v>
+      </c>
+      <c r="P27" t="str">
+        <f t="shared" si="7"/>
+        <v>#7C</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>199</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="1"/>
+        <v>#23</v>
+      </c>
+      <c r="E28" t="s">
+        <v>206</v>
+      </c>
+      <c r="F28" t="s">
+        <v>82</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="2"/>
+        <v>#DF</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="3"/>
+        <v>#7C</v>
+      </c>
+      <c r="I28" t="s">
+        <v>3</v>
+      </c>
+      <c r="J28" t="s">
+        <v>8</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L28" t="str">
+        <f t="shared" si="5"/>
+        <v>#01</v>
+      </c>
+      <c r="M28" t="s">
+        <v>14</v>
+      </c>
+      <c r="N28" t="s">
+        <v>79</v>
+      </c>
+      <c r="O28" t="str">
+        <f t="shared" si="6"/>
+        <v>#FE</v>
+      </c>
+      <c r="P28" t="str">
+        <f t="shared" si="7"/>
+        <v>#38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="1"/>
+        <v>#03</v>
+      </c>
+      <c r="E29" t="s">
+        <v>206</v>
+      </c>
+      <c r="F29" t="s">
+        <v>79</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="2"/>
+        <v>#DF</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="3"/>
+        <v>#38</v>
+      </c>
+      <c r="I29" t="s">
+        <v>3</v>
+      </c>
+      <c r="J29" t="s">
+        <v>8</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L29" t="str">
+        <f t="shared" si="5"/>
+        <v>#01</v>
+      </c>
+      <c r="M29" t="s">
+        <v>207</v>
+      </c>
+      <c r="N29" t="s">
+        <v>3</v>
+      </c>
+      <c r="O29" t="str">
+        <f t="shared" si="6"/>
+        <v>#DE</v>
+      </c>
+      <c r="P29" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="1"/>
+        <v>#07</v>
+      </c>
+      <c r="E30" t="s">
+        <v>70</v>
+      </c>
+      <c r="F30" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="2"/>
+        <v>#9F</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I30" t="s">
+        <v>3</v>
+      </c>
+      <c r="J30" t="s">
+        <v>8</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L30" t="str">
+        <f t="shared" si="5"/>
+        <v>#01</v>
+      </c>
+      <c r="M30" t="s">
+        <v>59</v>
+      </c>
+      <c r="N30" t="s">
+        <v>3</v>
+      </c>
+      <c r="O30" t="str">
+        <f t="shared" si="6"/>
+        <v>#CE</v>
+      </c>
+      <c r="P30" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="1"/>
+        <v>#07</v>
+      </c>
+      <c r="E31" t="s">
+        <v>62</v>
+      </c>
+      <c r="F31" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="2"/>
+        <v>#8E</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I31" t="s">
+        <v>3</v>
+      </c>
+      <c r="J31" t="s">
+        <v>8</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L31" t="str">
+        <f t="shared" si="5"/>
+        <v>#01</v>
+      </c>
+      <c r="M31" t="s">
+        <v>59</v>
+      </c>
+      <c r="N31" t="s">
+        <v>3</v>
+      </c>
+      <c r="O31" t="str">
+        <f t="shared" si="6"/>
+        <v>#CE</v>
+      </c>
+      <c r="P31" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="1"/>
+        <v>#0F</v>
+      </c>
+      <c r="E32" t="s">
+        <v>251</v>
+      </c>
+      <c r="F32" t="s">
+        <v>3</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="2"/>
+        <v>#8F</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I32" t="s">
+        <v>3</v>
+      </c>
+      <c r="J32" t="s">
+        <v>11</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L32" t="str">
+        <f t="shared" si="5"/>
+        <v>#03</v>
+      </c>
+      <c r="M32" t="s">
+        <v>207</v>
+      </c>
+      <c r="N32" t="s">
+        <v>3</v>
+      </c>
+      <c r="O32" t="str">
+        <f t="shared" si="6"/>
+        <v>#DE</v>
+      </c>
+      <c r="P32" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s">
+        <v>153</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="1"/>
+        <v>#1F</v>
+      </c>
+      <c r="E33" t="s">
+        <v>153</v>
+      </c>
+      <c r="F33" t="s">
+        <v>3</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="2"/>
+        <v>#1F</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I33" t="s">
+        <v>3</v>
+      </c>
+      <c r="J33" t="s">
+        <v>71</v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L33" t="str">
+        <f t="shared" si="5"/>
+        <v>#0F</v>
+      </c>
+      <c r="M33" t="s">
+        <v>14</v>
+      </c>
+      <c r="N33" t="s">
+        <v>3</v>
+      </c>
+      <c r="O33" t="str">
+        <f t="shared" ref="O33" si="8">CONCATENATE("#",BIN2HEX(REPLACE(M33,1,1,""),2))</f>
+        <v>#FE</v>
+      </c>
+      <c r="P33" t="str">
+        <f t="shared" ref="P33" si="9">CONCATENATE("#",BIN2HEX(REPLACE(N33,1,1,""),2))</f>
         <v>#00</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fin sprite jefe zombi
</commit_message>
<xml_diff>
--- a/doc/diseño sprites/diseno sprites.xlsx
+++ b/doc/diseño sprites/diseno sprites.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="6" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="8" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="zombi" sheetId="1" r:id="rId1"/>
@@ -25,6 +25,8 @@
     <sheet name="manos" sheetId="11" r:id="rId11"/>
     <sheet name="jefecaballerod" sheetId="12" r:id="rId12"/>
     <sheet name="jefecaballeroi" sheetId="13" r:id="rId13"/>
+    <sheet name="jefezombid" sheetId="14" r:id="rId14"/>
+    <sheet name="jefezombii" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2690" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3202" uniqueCount="303">
   <si>
     <t>00011111n</t>
   </si>
@@ -939,6 +941,12 @@
   </si>
   <si>
     <t>n11110100</t>
+  </si>
+  <si>
+    <t>n10101100</t>
+  </si>
+  <si>
+    <t>n10010110</t>
   </si>
 </sst>
 </file>
@@ -5201,7 +5209,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -8932,6 +8940,3748 @@
       <c r="P33" t="str">
         <f t="shared" ref="P33" si="9">CONCATENATE("#",BIN2HEX(REPLACE(N33,1,1,""),2))</f>
         <v>#00</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P17" sqref="O17:P17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(A1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="D1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(B1,1,1,""),2))</f>
+        <v>#01</v>
+      </c>
+      <c r="E1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(E1,1,1,""),2))</f>
+        <v>#10</v>
+      </c>
+      <c r="H1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(F1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(I1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="L1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(J1,1,1,""),2))</f>
+        <v>#01</v>
+      </c>
+      <c r="M1" t="s">
+        <v>234</v>
+      </c>
+      <c r="N1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(M1,1,1,""),2))</f>
+        <v>#10</v>
+      </c>
+      <c r="P1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(N1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C33" si="0">CONCATENATE("#",BIN2HEX(REPLACE(A2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D33" si="1">CONCATENATE("#",BIN2HEX(REPLACE(B2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G33" si="2">CONCATENATE("#",BIN2HEX(REPLACE(E2,1,1,""),2))</f>
+        <v>#FC</v>
+      </c>
+      <c r="H2" t="str">
+        <f t="shared" ref="H2:H33" si="3">CONCATENATE("#",BIN2HEX(REPLACE(F2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" t="str">
+        <f t="shared" ref="K2:K33" si="4">CONCATENATE("#",BIN2HEX(REPLACE(I2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="L2" t="str">
+        <f t="shared" ref="L2:L33" si="5">CONCATENATE("#",BIN2HEX(REPLACE(J2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="M2" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" t="str">
+        <f t="shared" ref="O2:O33" si="6">CONCATENATE("#",BIN2HEX(REPLACE(M2,1,1,""),2))</f>
+        <v>#FC</v>
+      </c>
+      <c r="P2" t="str">
+        <f t="shared" ref="P2:P33" si="7">CONCATENATE("#",BIN2HEX(REPLACE(N2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="1"/>
+        <v>#00</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="2"/>
+        <v>#FC</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" si="5"/>
+        <v>#00</v>
+      </c>
+      <c r="M3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3" t="str">
+        <f t="shared" si="6"/>
+        <v>#FC</v>
+      </c>
+      <c r="P3" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v>#01</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="2"/>
+        <v>#F8</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="5"/>
+        <v>#01</v>
+      </c>
+      <c r="M4" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O4" t="str">
+        <f t="shared" si="6"/>
+        <v>#F8</v>
+      </c>
+      <c r="P4" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v>#01</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>76</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="2"/>
+        <v>#FE</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="3"/>
+        <v>#C0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>3</v>
+      </c>
+      <c r="J5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="5"/>
+        <v>#01</v>
+      </c>
+      <c r="M5" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" t="s">
+        <v>76</v>
+      </c>
+      <c r="O5" t="str">
+        <f t="shared" si="6"/>
+        <v>#FE</v>
+      </c>
+      <c r="P5" t="str">
+        <f t="shared" si="7"/>
+        <v>#C0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="1"/>
+        <v>#01</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" t="s">
+        <v>76</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="3"/>
+        <v>#C0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="5"/>
+        <v>#01</v>
+      </c>
+      <c r="M6" t="s">
+        <v>35</v>
+      </c>
+      <c r="N6" t="s">
+        <v>76</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P6" t="str">
+        <f t="shared" si="7"/>
+        <v>#C0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="1"/>
+        <v>#01</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="3"/>
+        <v>#E0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>3</v>
+      </c>
+      <c r="J7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="5"/>
+        <v>#01</v>
+      </c>
+      <c r="M7" t="s">
+        <v>35</v>
+      </c>
+      <c r="N7" t="s">
+        <v>33</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P7" t="str">
+        <f t="shared" si="7"/>
+        <v>#E0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v>#01</v>
+      </c>
+      <c r="E8" t="s">
+        <v>154</v>
+      </c>
+      <c r="F8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="2"/>
+        <v>#E3</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="3"/>
+        <v>#80</v>
+      </c>
+      <c r="I8" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="5"/>
+        <v>#01</v>
+      </c>
+      <c r="M8" t="s">
+        <v>154</v>
+      </c>
+      <c r="N8" t="s">
+        <v>101</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="6"/>
+        <v>#E3</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" si="7"/>
+        <v>#80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="1"/>
+        <v>#7E</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="3"/>
+        <v>#E0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>3</v>
+      </c>
+      <c r="J9" t="s">
+        <v>46</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="5"/>
+        <v>#7E</v>
+      </c>
+      <c r="M9" t="s">
+        <v>35</v>
+      </c>
+      <c r="N9" t="s">
+        <v>33</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" si="7"/>
+        <v>#E0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="1"/>
+        <v>#7F</v>
+      </c>
+      <c r="E10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="2"/>
+        <v>#7F</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="3"/>
+        <v>#E0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>3</v>
+      </c>
+      <c r="J10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="5"/>
+        <v>#7F</v>
+      </c>
+      <c r="M10" t="s">
+        <v>37</v>
+      </c>
+      <c r="N10" t="s">
+        <v>33</v>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" si="6"/>
+        <v>#7F</v>
+      </c>
+      <c r="P10" t="str">
+        <f t="shared" si="7"/>
+        <v>#E0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>#03</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
+      <c r="E11" t="s">
+        <v>237</v>
+      </c>
+      <c r="F11" t="s">
+        <v>33</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="2"/>
+        <v>#BF</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="3"/>
+        <v>#E0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" t="s">
+        <v>35</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="4"/>
+        <v>#03</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M11" t="s">
+        <v>20</v>
+      </c>
+      <c r="N11" t="s">
+        <v>169</v>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" si="6"/>
+        <v>#BC</v>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" si="7"/>
+        <v>#60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>#0F</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
+      <c r="E12" t="s">
+        <v>206</v>
+      </c>
+      <c r="F12" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="2"/>
+        <v>#DF</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="3"/>
+        <v>#C0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>71</v>
+      </c>
+      <c r="J12" t="s">
+        <v>35</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="4"/>
+        <v>#0F</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M12" t="s">
+        <v>57</v>
+      </c>
+      <c r="N12" t="s">
+        <v>39</v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" si="6"/>
+        <v>#DC</v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" si="7"/>
+        <v>#40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>#3F</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="2"/>
+        <v>#E0</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I13" t="s">
+        <v>218</v>
+      </c>
+      <c r="J13" t="s">
+        <v>35</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="4"/>
+        <v>#17</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M13" t="s">
+        <v>33</v>
+      </c>
+      <c r="N13" t="s">
+        <v>3</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" si="6"/>
+        <v>#E0</v>
+      </c>
+      <c r="P13" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>#08</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>#7F</v>
+      </c>
+      <c r="E14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="3"/>
+        <v>#C0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>104</v>
+      </c>
+      <c r="J14" t="s">
+        <v>37</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="4"/>
+        <v>#28</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="5"/>
+        <v>#7F</v>
+      </c>
+      <c r="M14" t="s">
+        <v>35</v>
+      </c>
+      <c r="N14" t="s">
+        <v>101</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P14" t="str">
+        <f t="shared" si="7"/>
+        <v>#80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" t="s">
+        <v>234</v>
+      </c>
+      <c r="B15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>#10</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>#0F</v>
+      </c>
+      <c r="E15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="3"/>
+        <v>#E0</v>
+      </c>
+      <c r="I15" t="s">
+        <v>234</v>
+      </c>
+      <c r="J15" t="s">
+        <v>71</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="4"/>
+        <v>#10</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="5"/>
+        <v>#0F</v>
+      </c>
+      <c r="M15" t="s">
+        <v>35</v>
+      </c>
+      <c r="N15" t="s">
+        <v>76</v>
+      </c>
+      <c r="O15" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P15" t="str">
+        <f t="shared" si="7"/>
+        <v>#C0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>#20</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>#3F</v>
+      </c>
+      <c r="E16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="3"/>
+        <v>#E0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>3</v>
+      </c>
+      <c r="J16" t="s">
+        <v>43</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="5"/>
+        <v>#3F</v>
+      </c>
+      <c r="M16" t="s">
+        <v>35</v>
+      </c>
+      <c r="N16" t="s">
+        <v>33</v>
+      </c>
+      <c r="O16" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P16" t="str">
+        <f t="shared" si="7"/>
+        <v>#E0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="1"/>
+        <v>#3F</v>
+      </c>
+      <c r="E18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="3"/>
+        <v>#E0</v>
+      </c>
+      <c r="I18" t="s">
+        <v>234</v>
+      </c>
+      <c r="J18" t="s">
+        <v>43</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="4"/>
+        <v>#10</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="5"/>
+        <v>#3F</v>
+      </c>
+      <c r="M18" t="s">
+        <v>35</v>
+      </c>
+      <c r="N18" t="s">
+        <v>33</v>
+      </c>
+      <c r="O18" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P18" t="str">
+        <f t="shared" si="7"/>
+        <v>#E0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19" t="s">
+        <v>234</v>
+      </c>
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>#10</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="1"/>
+        <v>#3F</v>
+      </c>
+      <c r="E19" t="s">
+        <v>152</v>
+      </c>
+      <c r="F19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="2"/>
+        <v>#FD</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="3"/>
+        <v>#F8</v>
+      </c>
+      <c r="I19" t="s">
+        <v>3</v>
+      </c>
+      <c r="J19" t="s">
+        <v>43</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="5"/>
+        <v>#3F</v>
+      </c>
+      <c r="M19" t="s">
+        <v>35</v>
+      </c>
+      <c r="N19" t="s">
+        <v>33</v>
+      </c>
+      <c r="O19" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P19" t="str">
+        <f t="shared" si="7"/>
+        <v>#E0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="1"/>
+        <v>#7F</v>
+      </c>
+      <c r="E20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="2"/>
+        <v>#F0</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="3"/>
+        <v>#78</v>
+      </c>
+      <c r="I20" t="s">
+        <v>234</v>
+      </c>
+      <c r="J20" t="s">
+        <v>37</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="4"/>
+        <v>#10</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="5"/>
+        <v>#7F</v>
+      </c>
+      <c r="M20" t="s">
+        <v>249</v>
+      </c>
+      <c r="N20" t="s">
+        <v>33</v>
+      </c>
+      <c r="O20" t="str">
+        <f t="shared" si="6"/>
+        <v>#F1</v>
+      </c>
+      <c r="P20" t="str">
+        <f t="shared" si="7"/>
+        <v>#E0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>#20</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
+      <c r="E21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="2"/>
+        <v>#F0</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="3"/>
+        <v>#78</v>
+      </c>
+      <c r="I21" t="s">
+        <v>3</v>
+      </c>
+      <c r="J21" t="s">
+        <v>35</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M21" t="s">
+        <v>249</v>
+      </c>
+      <c r="N21" t="s">
+        <v>33</v>
+      </c>
+      <c r="O21" t="str">
+        <f t="shared" si="6"/>
+        <v>#F1</v>
+      </c>
+      <c r="P21" t="str">
+        <f t="shared" si="7"/>
+        <v>#E0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>#01</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
+      <c r="E22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" t="s">
+        <v>82</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="2"/>
+        <v>#F0</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="3"/>
+        <v>#7C</v>
+      </c>
+      <c r="I22" t="s">
+        <v>293</v>
+      </c>
+      <c r="J22" t="s">
+        <v>35</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="4"/>
+        <v>#41</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M22" t="s">
+        <v>249</v>
+      </c>
+      <c r="N22" t="s">
+        <v>9</v>
+      </c>
+      <c r="O22" t="str">
+        <f t="shared" si="6"/>
+        <v>#F1</v>
+      </c>
+      <c r="P22" t="str">
+        <f t="shared" si="7"/>
+        <v>#F0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>#03</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
+      <c r="E23" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" t="s">
+        <v>43</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="2"/>
+        <v>#E0</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="3"/>
+        <v>#3F</v>
+      </c>
+      <c r="I23" t="s">
+        <v>217</v>
+      </c>
+      <c r="J23" t="s">
+        <v>35</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="4"/>
+        <v>#11</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M23" t="s">
+        <v>33</v>
+      </c>
+      <c r="N23" t="s">
+        <v>7</v>
+      </c>
+      <c r="O23" t="str">
+        <f t="shared" si="6"/>
+        <v>#E0</v>
+      </c>
+      <c r="P23" t="str">
+        <f t="shared" si="7"/>
+        <v>#FC</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" t="s">
+        <v>228</v>
+      </c>
+      <c r="B24" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>#13</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
+      <c r="E24" t="s">
+        <v>33</v>
+      </c>
+      <c r="F24" t="s">
+        <v>263</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="2"/>
+        <v>#E0</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="3"/>
+        <v>#2B</v>
+      </c>
+      <c r="I24" t="s">
+        <v>8</v>
+      </c>
+      <c r="J24" t="s">
+        <v>35</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="4"/>
+        <v>#01</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M24" t="s">
+        <v>33</v>
+      </c>
+      <c r="N24" t="s">
+        <v>301</v>
+      </c>
+      <c r="O24" t="str">
+        <f t="shared" si="6"/>
+        <v>#E0</v>
+      </c>
+      <c r="P24" t="str">
+        <f t="shared" si="7"/>
+        <v>#AC</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>#03</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
+      <c r="E25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" t="s">
+        <v>262</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="2"/>
+        <v>#F0</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="3"/>
+        <v>#69</v>
+      </c>
+      <c r="I25" t="s">
+        <v>8</v>
+      </c>
+      <c r="J25" t="s">
+        <v>35</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="4"/>
+        <v>#01</v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M25" t="s">
+        <v>249</v>
+      </c>
+      <c r="N25" t="s">
+        <v>225</v>
+      </c>
+      <c r="O25" t="str">
+        <f t="shared" si="6"/>
+        <v>#F1</v>
+      </c>
+      <c r="P25" t="str">
+        <f t="shared" si="7"/>
+        <v>#A4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>#0F</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="1"/>
+        <v>#E0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" t="s">
+        <v>78</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="2"/>
+        <v>#FC</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="3"/>
+        <v>#0C</v>
+      </c>
+      <c r="I26" t="s">
+        <v>55</v>
+      </c>
+      <c r="J26" t="s">
+        <v>37</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="4"/>
+        <v>#20</v>
+      </c>
+      <c r="L26" t="str">
+        <f t="shared" si="5"/>
+        <v>#7F</v>
+      </c>
+      <c r="M26" t="s">
+        <v>7</v>
+      </c>
+      <c r="N26" t="s">
+        <v>31</v>
+      </c>
+      <c r="O26" t="str">
+        <f t="shared" si="6"/>
+        <v>#FC</v>
+      </c>
+      <c r="P26" t="str">
+        <f t="shared" si="7"/>
+        <v>#30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" t="s">
+        <v>153</v>
+      </c>
+      <c r="B27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>#1F</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="1"/>
+        <v>#C0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>82</v>
+      </c>
+      <c r="F27" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="2"/>
+        <v>#7C</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I27" t="s">
+        <v>3</v>
+      </c>
+      <c r="J27" t="s">
+        <v>14</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L27" t="str">
+        <f t="shared" si="5"/>
+        <v>#FE</v>
+      </c>
+      <c r="M27" t="s">
+        <v>82</v>
+      </c>
+      <c r="N27" t="s">
+        <v>3</v>
+      </c>
+      <c r="O27" t="str">
+        <f t="shared" si="6"/>
+        <v>#7C</v>
+      </c>
+      <c r="P27" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" t="s">
+        <v>147</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>#1E</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="1"/>
+        <v>#00</v>
+      </c>
+      <c r="E28" t="s">
+        <v>23</v>
+      </c>
+      <c r="F28" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="2"/>
+        <v>#3C</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I28" t="s">
+        <v>234</v>
+      </c>
+      <c r="J28" t="s">
+        <v>9</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="4"/>
+        <v>#10</v>
+      </c>
+      <c r="L28" t="str">
+        <f t="shared" si="5"/>
+        <v>#F0</v>
+      </c>
+      <c r="M28" t="s">
+        <v>23</v>
+      </c>
+      <c r="N28" t="s">
+        <v>3</v>
+      </c>
+      <c r="O28" t="str">
+        <f t="shared" si="6"/>
+        <v>#3C</v>
+      </c>
+      <c r="P28" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>#3E</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="1"/>
+        <v>#00</v>
+      </c>
+      <c r="E29" t="s">
+        <v>80</v>
+      </c>
+      <c r="F29" t="s">
+        <v>3</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="2"/>
+        <v>#3E</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I29" t="s">
+        <v>8</v>
+      </c>
+      <c r="J29" t="s">
+        <v>9</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="4"/>
+        <v>#01</v>
+      </c>
+      <c r="L29" t="str">
+        <f t="shared" si="5"/>
+        <v>#F0</v>
+      </c>
+      <c r="M29" t="s">
+        <v>80</v>
+      </c>
+      <c r="N29" t="s">
+        <v>3</v>
+      </c>
+      <c r="O29" t="str">
+        <f t="shared" si="6"/>
+        <v>#3E</v>
+      </c>
+      <c r="P29" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>#3C</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="1"/>
+        <v>#00</v>
+      </c>
+      <c r="E30" t="s">
+        <v>147</v>
+      </c>
+      <c r="F30" t="s">
+        <v>3</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="2"/>
+        <v>#1E</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I30" t="s">
+        <v>8</v>
+      </c>
+      <c r="J30" t="s">
+        <v>33</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="4"/>
+        <v>#01</v>
+      </c>
+      <c r="L30" t="str">
+        <f t="shared" si="5"/>
+        <v>#E0</v>
+      </c>
+      <c r="M30" t="s">
+        <v>147</v>
+      </c>
+      <c r="N30" t="s">
+        <v>3</v>
+      </c>
+      <c r="O30" t="str">
+        <f t="shared" si="6"/>
+        <v>#1E</v>
+      </c>
+      <c r="P30" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>#3C</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="1"/>
+        <v>#00</v>
+      </c>
+      <c r="E31" t="s">
+        <v>147</v>
+      </c>
+      <c r="F31" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="2"/>
+        <v>#1E</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I31" t="s">
+        <v>8</v>
+      </c>
+      <c r="J31" t="s">
+        <v>33</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="4"/>
+        <v>#01</v>
+      </c>
+      <c r="L31" t="str">
+        <f t="shared" si="5"/>
+        <v>#E0</v>
+      </c>
+      <c r="M31" t="s">
+        <v>147</v>
+      </c>
+      <c r="N31" t="s">
+        <v>3</v>
+      </c>
+      <c r="O31" t="str">
+        <f t="shared" si="6"/>
+        <v>#1E</v>
+      </c>
+      <c r="P31" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>#7C</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="1"/>
+        <v>#00</v>
+      </c>
+      <c r="E32" t="s">
+        <v>80</v>
+      </c>
+      <c r="F32" t="s">
+        <v>3</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="2"/>
+        <v>#3E</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I32" t="s">
+        <v>11</v>
+      </c>
+      <c r="J32" t="s">
+        <v>33</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="4"/>
+        <v>#03</v>
+      </c>
+      <c r="L32" t="str">
+        <f t="shared" si="5"/>
+        <v>#E0</v>
+      </c>
+      <c r="M32" t="s">
+        <v>80</v>
+      </c>
+      <c r="N32" t="s">
+        <v>3</v>
+      </c>
+      <c r="O32" t="str">
+        <f t="shared" si="6"/>
+        <v>#3E</v>
+      </c>
+      <c r="P32" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>#F8</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="1"/>
+        <v>#00</v>
+      </c>
+      <c r="E33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" t="s">
+        <v>3</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="2"/>
+        <v>#FE</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I33" t="s">
+        <v>15</v>
+      </c>
+      <c r="J33" t="s">
+        <v>76</v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="4"/>
+        <v>#07</v>
+      </c>
+      <c r="L33" t="str">
+        <f t="shared" si="5"/>
+        <v>#C0</v>
+      </c>
+      <c r="M33" t="s">
+        <v>14</v>
+      </c>
+      <c r="N33" t="s">
+        <v>3</v>
+      </c>
+      <c r="O33" t="str">
+        <f t="shared" si="6"/>
+        <v>#FE</v>
+      </c>
+      <c r="P33" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(A1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="D1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(B1,1,1,""),2))</f>
+        <v>#08</v>
+      </c>
+      <c r="E1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(E1,1,1,""),2))</f>
+        <v>#80</v>
+      </c>
+      <c r="H1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(F1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(I1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="L1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(J1,1,1,""),2))</f>
+        <v>#08</v>
+      </c>
+      <c r="M1" t="s">
+        <v>101</v>
+      </c>
+      <c r="N1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(M1,1,1,""),2))</f>
+        <v>#80</v>
+      </c>
+      <c r="P1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(N1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C33" si="0">CONCATENATE("#",BIN2HEX(REPLACE(A2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D33" si="1">CONCATENATE("#",BIN2HEX(REPLACE(B2,1,1,""),2))</f>
+        <v>#3F</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G33" si="2">CONCATENATE("#",BIN2HEX(REPLACE(E2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="H2" t="str">
+        <f t="shared" ref="H2:H33" si="3">CONCATENATE("#",BIN2HEX(REPLACE(F2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" t="str">
+        <f t="shared" ref="K2:K33" si="4">CONCATENATE("#",BIN2HEX(REPLACE(I2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="L2" t="str">
+        <f t="shared" ref="L2:L33" si="5">CONCATENATE("#",BIN2HEX(REPLACE(J2,1,1,""),2))</f>
+        <v>#3F</v>
+      </c>
+      <c r="M2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" t="str">
+        <f t="shared" ref="O2:O33" si="6">CONCATENATE("#",BIN2HEX(REPLACE(M2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="P2" t="str">
+        <f t="shared" ref="P2:P33" si="7">CONCATENATE("#",BIN2HEX(REPLACE(N2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="1"/>
+        <v>#3F</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="2"/>
+        <v>#00</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" si="5"/>
+        <v>#3F</v>
+      </c>
+      <c r="M3" t="s">
+        <v>3</v>
+      </c>
+      <c r="N3" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3" t="str">
+        <f t="shared" si="6"/>
+        <v>#00</v>
+      </c>
+      <c r="P3" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v>#1F</v>
+      </c>
+      <c r="E4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="2"/>
+        <v>#80</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>153</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="5"/>
+        <v>#1F</v>
+      </c>
+      <c r="M4" t="s">
+        <v>101</v>
+      </c>
+      <c r="N4" t="s">
+        <v>3</v>
+      </c>
+      <c r="O4" t="str">
+        <f t="shared" si="6"/>
+        <v>#80</v>
+      </c>
+      <c r="P4" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>#03</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v>#7F</v>
+      </c>
+      <c r="E5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="2"/>
+        <v>#80</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="4"/>
+        <v>#03</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="5"/>
+        <v>#7F</v>
+      </c>
+      <c r="M5" t="s">
+        <v>101</v>
+      </c>
+      <c r="N5" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" t="str">
+        <f t="shared" si="6"/>
+        <v>#80</v>
+      </c>
+      <c r="P5" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>#03</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
+      <c r="E6" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="2"/>
+        <v>#80</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="4"/>
+        <v>#03</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M6" t="s">
+        <v>101</v>
+      </c>
+      <c r="N6" t="s">
+        <v>3</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" si="6"/>
+        <v>#80</v>
+      </c>
+      <c r="P6" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>#07</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
+      <c r="E7" t="s">
+        <v>101</v>
+      </c>
+      <c r="F7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="2"/>
+        <v>#80</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J7" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="4"/>
+        <v>#07</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M7" t="s">
+        <v>101</v>
+      </c>
+      <c r="N7" t="s">
+        <v>3</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="6"/>
+        <v>#80</v>
+      </c>
+      <c r="P7" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>#01</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v>#C7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="2"/>
+        <v>#80</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" t="s">
+        <v>94</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="4"/>
+        <v>#01</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="5"/>
+        <v>#C7</v>
+      </c>
+      <c r="M8" t="s">
+        <v>101</v>
+      </c>
+      <c r="N8" t="s">
+        <v>3</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="6"/>
+        <v>#80</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>#07</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="2"/>
+        <v>#7E</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I9" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" t="s">
+        <v>35</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="4"/>
+        <v>#07</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M9" t="s">
+        <v>46</v>
+      </c>
+      <c r="N9" t="s">
+        <v>3</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="6"/>
+        <v>#7E</v>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>#07</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="1"/>
+        <v>#FE</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="2"/>
+        <v>#FE</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I10" t="s">
+        <v>15</v>
+      </c>
+      <c r="J10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="4"/>
+        <v>#07</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="5"/>
+        <v>#FE</v>
+      </c>
+      <c r="M10" t="s">
+        <v>14</v>
+      </c>
+      <c r="N10" t="s">
+        <v>3</v>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" si="6"/>
+        <v>#FE</v>
+      </c>
+      <c r="P10" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>152</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>#07</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v>#FD</v>
+      </c>
+      <c r="E11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="3"/>
+        <v>#C0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>156</v>
+      </c>
+      <c r="J11" t="s">
+        <v>215</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="4"/>
+        <v>#06</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="5"/>
+        <v>#3D</v>
+      </c>
+      <c r="M11" t="s">
+        <v>35</v>
+      </c>
+      <c r="N11" t="s">
+        <v>76</v>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" si="7"/>
+        <v>#C0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>227</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>#03</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v>#FB</v>
+      </c>
+      <c r="E12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="3"/>
+        <v>#F0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" t="s">
+        <v>250</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="4"/>
+        <v>#02</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="5"/>
+        <v>#3B</v>
+      </c>
+      <c r="M12" t="s">
+        <v>35</v>
+      </c>
+      <c r="N12" t="s">
+        <v>9</v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" si="7"/>
+        <v>#F0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v>#07</v>
+      </c>
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="3"/>
+        <v>#FC</v>
+      </c>
+      <c r="I13" t="s">
+        <v>3</v>
+      </c>
+      <c r="J13" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="5"/>
+        <v>#07</v>
+      </c>
+      <c r="M13" t="s">
+        <v>35</v>
+      </c>
+      <c r="N13" t="s">
+        <v>209</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P13" t="str">
+        <f t="shared" si="7"/>
+        <v>#E8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>#FC</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
+      <c r="E14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" t="s">
+        <v>234</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="2"/>
+        <v>#FE</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="3"/>
+        <v>#10</v>
+      </c>
+      <c r="I14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J14" t="s">
+        <v>35</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="4"/>
+        <v>#01</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M14" t="s">
+        <v>14</v>
+      </c>
+      <c r="N14" t="s">
+        <v>106</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="6"/>
+        <v>#FE</v>
+      </c>
+      <c r="P14" t="str">
+        <f t="shared" si="7"/>
+        <v>#14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>#07</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>103</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="2"/>
+        <v>#F0</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="3"/>
+        <v>#08</v>
+      </c>
+      <c r="I15" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" t="s">
+        <v>35</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="4"/>
+        <v>#03</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M15" t="s">
+        <v>9</v>
+      </c>
+      <c r="N15" t="s">
+        <v>103</v>
+      </c>
+      <c r="O15" t="str">
+        <f t="shared" si="6"/>
+        <v>#F0</v>
+      </c>
+      <c r="P15" t="str">
+        <f t="shared" si="7"/>
+        <v>#08</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>#07</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" t="s">
+        <v>216</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="2"/>
+        <v>#FC</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="3"/>
+        <v>#04</v>
+      </c>
+      <c r="I16" t="s">
+        <v>15</v>
+      </c>
+      <c r="J16" t="s">
+        <v>35</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="4"/>
+        <v>#07</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M16" t="s">
+        <v>7</v>
+      </c>
+      <c r="N16" t="s">
+        <v>3</v>
+      </c>
+      <c r="O16" t="str">
+        <f t="shared" si="6"/>
+        <v>#FC</v>
+      </c>
+      <c r="P16" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>#07</v>
+      </c>
+      <c r="D18" t="str">
+        <f t="shared" si="1"/>
+        <v>#FF</v>
+      </c>
+      <c r="E18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" t="str">
+        <f t="shared" si="2"/>
+        <v>#FC</v>
+      </c>
+      <c r="H18" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I18" t="s">
+        <v>15</v>
+      </c>
+      <c r="J18" t="s">
+        <v>35</v>
+      </c>
+      <c r="K18" t="str">
+        <f t="shared" si="4"/>
+        <v>#07</v>
+      </c>
+      <c r="L18" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M18" t="s">
+        <v>7</v>
+      </c>
+      <c r="N18" t="s">
+        <v>103</v>
+      </c>
+      <c r="O18" t="str">
+        <f t="shared" si="6"/>
+        <v>#FC</v>
+      </c>
+      <c r="P18" t="str">
+        <f t="shared" si="7"/>
+        <v>#08</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19" t="s">
+        <v>153</v>
+      </c>
+      <c r="B19" t="s">
+        <v>237</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>#1F</v>
+      </c>
+      <c r="D19" t="str">
+        <f t="shared" si="1"/>
+        <v>#BF</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" t="s">
+        <v>103</v>
+      </c>
+      <c r="G19" t="str">
+        <f t="shared" si="2"/>
+        <v>#FC</v>
+      </c>
+      <c r="H19" t="str">
+        <f t="shared" si="3"/>
+        <v>#08</v>
+      </c>
+      <c r="I19" t="s">
+        <v>15</v>
+      </c>
+      <c r="J19" t="s">
+        <v>35</v>
+      </c>
+      <c r="K19" t="str">
+        <f t="shared" si="4"/>
+        <v>#07</v>
+      </c>
+      <c r="L19" t="str">
+        <f t="shared" si="5"/>
+        <v>#FF</v>
+      </c>
+      <c r="M19" t="s">
+        <v>7</v>
+      </c>
+      <c r="N19" t="s">
+        <v>3</v>
+      </c>
+      <c r="O19" t="str">
+        <f t="shared" si="6"/>
+        <v>#FC</v>
+      </c>
+      <c r="P19" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" t="s">
+        <v>147</v>
+      </c>
+      <c r="B20" t="s">
+        <v>71</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>#1E</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="1"/>
+        <v>#0F</v>
+      </c>
+      <c r="E20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" t="str">
+        <f t="shared" si="2"/>
+        <v>#FE</v>
+      </c>
+      <c r="H20" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I20" t="s">
+        <v>15</v>
+      </c>
+      <c r="J20" t="s">
+        <v>251</v>
+      </c>
+      <c r="K20" t="str">
+        <f t="shared" si="4"/>
+        <v>#07</v>
+      </c>
+      <c r="L20" t="str">
+        <f t="shared" si="5"/>
+        <v>#8F</v>
+      </c>
+      <c r="M20" t="s">
+        <v>14</v>
+      </c>
+      <c r="N20" t="s">
+        <v>103</v>
+      </c>
+      <c r="O20" t="str">
+        <f t="shared" si="6"/>
+        <v>#FE</v>
+      </c>
+      <c r="P20" t="str">
+        <f t="shared" si="7"/>
+        <v>#08</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" t="s">
+        <v>147</v>
+      </c>
+      <c r="B21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>#1E</v>
+      </c>
+      <c r="D21" t="str">
+        <f t="shared" si="1"/>
+        <v>#0F</v>
+      </c>
+      <c r="E21" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" t="s">
+        <v>216</v>
+      </c>
+      <c r="G21" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H21" t="str">
+        <f t="shared" si="3"/>
+        <v>#04</v>
+      </c>
+      <c r="I21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J21" t="s">
+        <v>251</v>
+      </c>
+      <c r="K21" t="str">
+        <f t="shared" si="4"/>
+        <v>#07</v>
+      </c>
+      <c r="L21" t="str">
+        <f t="shared" si="5"/>
+        <v>#8F</v>
+      </c>
+      <c r="M21" t="s">
+        <v>35</v>
+      </c>
+      <c r="N21" t="s">
+        <v>3</v>
+      </c>
+      <c r="O21" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P21" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>#3E</v>
+      </c>
+      <c r="D22" t="str">
+        <f t="shared" si="1"/>
+        <v>#0F</v>
+      </c>
+      <c r="E22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" t="s">
+        <v>101</v>
+      </c>
+      <c r="G22" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H22" t="str">
+        <f t="shared" si="3"/>
+        <v>#80</v>
+      </c>
+      <c r="I22" t="s">
+        <v>71</v>
+      </c>
+      <c r="J22" t="s">
+        <v>251</v>
+      </c>
+      <c r="K22" t="str">
+        <f t="shared" si="4"/>
+        <v>#0F</v>
+      </c>
+      <c r="L22" t="str">
+        <f t="shared" si="5"/>
+        <v>#8F</v>
+      </c>
+      <c r="M22" t="s">
+        <v>35</v>
+      </c>
+      <c r="N22" t="s">
+        <v>159</v>
+      </c>
+      <c r="O22" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P22" t="str">
+        <f t="shared" si="7"/>
+        <v>#82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>#FC</v>
+      </c>
+      <c r="D23" t="str">
+        <f t="shared" si="1"/>
+        <v>#07</v>
+      </c>
+      <c r="E23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" t="s">
+        <v>76</v>
+      </c>
+      <c r="G23" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" si="3"/>
+        <v>#C0</v>
+      </c>
+      <c r="I23" t="s">
+        <v>43</v>
+      </c>
+      <c r="J23" t="s">
+        <v>15</v>
+      </c>
+      <c r="K23" t="str">
+        <f t="shared" si="4"/>
+        <v>#3F</v>
+      </c>
+      <c r="L23" t="str">
+        <f t="shared" si="5"/>
+        <v>#07</v>
+      </c>
+      <c r="M23" t="s">
+        <v>35</v>
+      </c>
+      <c r="N23" t="s">
+        <v>205</v>
+      </c>
+      <c r="O23" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P23" t="str">
+        <f t="shared" si="7"/>
+        <v>#88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" t="s">
+        <v>265</v>
+      </c>
+      <c r="B24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>#D4</v>
+      </c>
+      <c r="D24" t="str">
+        <f t="shared" si="1"/>
+        <v>#07</v>
+      </c>
+      <c r="E24" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" t="s">
+        <v>230</v>
+      </c>
+      <c r="G24" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" si="3"/>
+        <v>#C8</v>
+      </c>
+      <c r="I24" t="s">
+        <v>149</v>
+      </c>
+      <c r="J24" t="s">
+        <v>15</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" si="4"/>
+        <v>#35</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" si="5"/>
+        <v>#07</v>
+      </c>
+      <c r="M24" t="s">
+        <v>35</v>
+      </c>
+      <c r="N24" t="s">
+        <v>101</v>
+      </c>
+      <c r="O24" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P24" t="str">
+        <f t="shared" si="7"/>
+        <v>#80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" t="s">
+        <v>302</v>
+      </c>
+      <c r="B25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>#96</v>
+      </c>
+      <c r="D25" t="str">
+        <f t="shared" si="1"/>
+        <v>#0F</v>
+      </c>
+      <c r="E25" t="s">
+        <v>35</v>
+      </c>
+      <c r="F25" t="s">
+        <v>76</v>
+      </c>
+      <c r="G25" t="str">
+        <f t="shared" si="2"/>
+        <v>#FF</v>
+      </c>
+      <c r="H25" t="str">
+        <f t="shared" si="3"/>
+        <v>#C0</v>
+      </c>
+      <c r="I25" t="s">
+        <v>201</v>
+      </c>
+      <c r="J25" t="s">
+        <v>251</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="4"/>
+        <v>#25</v>
+      </c>
+      <c r="L25" t="str">
+        <f t="shared" si="5"/>
+        <v>#8F</v>
+      </c>
+      <c r="M25" t="s">
+        <v>35</v>
+      </c>
+      <c r="N25" t="s">
+        <v>101</v>
+      </c>
+      <c r="O25" t="str">
+        <f t="shared" si="6"/>
+        <v>#FF</v>
+      </c>
+      <c r="P25" t="str">
+        <f t="shared" si="7"/>
+        <v>#80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>#30</v>
+      </c>
+      <c r="D26" t="str">
+        <f t="shared" si="1"/>
+        <v>#3F</v>
+      </c>
+      <c r="E26" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" t="str">
+        <f t="shared" si="2"/>
+        <v>#07</v>
+      </c>
+      <c r="H26" t="str">
+        <f t="shared" si="3"/>
+        <v>#F0</v>
+      </c>
+      <c r="I26" t="s">
+        <v>78</v>
+      </c>
+      <c r="J26" t="s">
+        <v>43</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="4"/>
+        <v>#0C</v>
+      </c>
+      <c r="L26" t="str">
+        <f t="shared" si="5"/>
+        <v>#3F</v>
+      </c>
+      <c r="M26" t="s">
+        <v>14</v>
+      </c>
+      <c r="N26" t="s">
+        <v>216</v>
+      </c>
+      <c r="O26" t="str">
+        <f t="shared" si="6"/>
+        <v>#FE</v>
+      </c>
+      <c r="P26" t="str">
+        <f t="shared" si="7"/>
+        <v>#04</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D27" t="str">
+        <f t="shared" si="1"/>
+        <v>#3E</v>
+      </c>
+      <c r="E27" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" t="s">
+        <v>2</v>
+      </c>
+      <c r="G27" t="str">
+        <f t="shared" si="2"/>
+        <v>#03</v>
+      </c>
+      <c r="H27" t="str">
+        <f t="shared" si="3"/>
+        <v>#F8</v>
+      </c>
+      <c r="I27" t="s">
+        <v>3</v>
+      </c>
+      <c r="J27" t="s">
+        <v>80</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L27" t="str">
+        <f t="shared" si="5"/>
+        <v>#3E</v>
+      </c>
+      <c r="M27" t="s">
+        <v>37</v>
+      </c>
+      <c r="N27" t="s">
+        <v>3</v>
+      </c>
+      <c r="O27" t="str">
+        <f t="shared" si="6"/>
+        <v>#7F</v>
+      </c>
+      <c r="P27" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D28" t="str">
+        <f t="shared" si="1"/>
+        <v>#3C</v>
+      </c>
+      <c r="E28" t="s">
+        <v>3</v>
+      </c>
+      <c r="F28" t="s">
+        <v>27</v>
+      </c>
+      <c r="G28" t="str">
+        <f t="shared" si="2"/>
+        <v>#00</v>
+      </c>
+      <c r="H28" t="str">
+        <f t="shared" si="3"/>
+        <v>#78</v>
+      </c>
+      <c r="I28" t="s">
+        <v>3</v>
+      </c>
+      <c r="J28" t="s">
+        <v>23</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L28" t="str">
+        <f t="shared" si="5"/>
+        <v>#3C</v>
+      </c>
+      <c r="M28" t="s">
+        <v>71</v>
+      </c>
+      <c r="N28" t="s">
+        <v>103</v>
+      </c>
+      <c r="O28" t="str">
+        <f t="shared" si="6"/>
+        <v>#0F</v>
+      </c>
+      <c r="P28" t="str">
+        <f t="shared" si="7"/>
+        <v>#08</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="1"/>
+        <v>#7C</v>
+      </c>
+      <c r="E29" t="s">
+        <v>3</v>
+      </c>
+      <c r="F29" t="s">
+        <v>82</v>
+      </c>
+      <c r="G29" t="str">
+        <f t="shared" si="2"/>
+        <v>#00</v>
+      </c>
+      <c r="H29" t="str">
+        <f t="shared" si="3"/>
+        <v>#7C</v>
+      </c>
+      <c r="I29" t="s">
+        <v>3</v>
+      </c>
+      <c r="J29" t="s">
+        <v>82</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L29" t="str">
+        <f t="shared" si="5"/>
+        <v>#7C</v>
+      </c>
+      <c r="M29" t="s">
+        <v>71</v>
+      </c>
+      <c r="N29" t="s">
+        <v>101</v>
+      </c>
+      <c r="O29" t="str">
+        <f t="shared" si="6"/>
+        <v>#0F</v>
+      </c>
+      <c r="P29" t="str">
+        <f t="shared" si="7"/>
+        <v>#80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D30" t="str">
+        <f t="shared" si="1"/>
+        <v>#78</v>
+      </c>
+      <c r="E30" t="s">
+        <v>3</v>
+      </c>
+      <c r="F30" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30" t="str">
+        <f t="shared" si="2"/>
+        <v>#00</v>
+      </c>
+      <c r="H30" t="str">
+        <f t="shared" si="3"/>
+        <v>#3C</v>
+      </c>
+      <c r="I30" t="s">
+        <v>3</v>
+      </c>
+      <c r="J30" t="s">
+        <v>27</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L30" t="str">
+        <f t="shared" si="5"/>
+        <v>#78</v>
+      </c>
+      <c r="M30" t="s">
+        <v>15</v>
+      </c>
+      <c r="N30" t="s">
+        <v>101</v>
+      </c>
+      <c r="O30" t="str">
+        <f t="shared" si="6"/>
+        <v>#07</v>
+      </c>
+      <c r="P30" t="str">
+        <f t="shared" si="7"/>
+        <v>#80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D31" t="str">
+        <f t="shared" si="1"/>
+        <v>#78</v>
+      </c>
+      <c r="E31" t="s">
+        <v>3</v>
+      </c>
+      <c r="F31" t="s">
+        <v>23</v>
+      </c>
+      <c r="G31" t="str">
+        <f t="shared" si="2"/>
+        <v>#00</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="3"/>
+        <v>#3C</v>
+      </c>
+      <c r="I31" t="s">
+        <v>3</v>
+      </c>
+      <c r="J31" t="s">
+        <v>27</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L31" t="str">
+        <f t="shared" si="5"/>
+        <v>#78</v>
+      </c>
+      <c r="M31" t="s">
+        <v>15</v>
+      </c>
+      <c r="N31" t="s">
+        <v>101</v>
+      </c>
+      <c r="O31" t="str">
+        <f t="shared" si="6"/>
+        <v>#07</v>
+      </c>
+      <c r="P31" t="str">
+        <f t="shared" si="7"/>
+        <v>#80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="1"/>
+        <v>#7C</v>
+      </c>
+      <c r="E32" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32" t="s">
+        <v>80</v>
+      </c>
+      <c r="G32" t="str">
+        <f t="shared" si="2"/>
+        <v>#00</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="3"/>
+        <v>#3E</v>
+      </c>
+      <c r="I32" t="s">
+        <v>3</v>
+      </c>
+      <c r="J32" t="s">
+        <v>82</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L32" t="str">
+        <f t="shared" si="5"/>
+        <v>#7C</v>
+      </c>
+      <c r="M32" t="s">
+        <v>15</v>
+      </c>
+      <c r="N32" t="s">
+        <v>76</v>
+      </c>
+      <c r="O32" t="str">
+        <f t="shared" si="6"/>
+        <v>#07</v>
+      </c>
+      <c r="P32" t="str">
+        <f t="shared" si="7"/>
+        <v>#C0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="1"/>
+        <v>#7F</v>
+      </c>
+      <c r="E33" t="s">
+        <v>3</v>
+      </c>
+      <c r="F33" t="s">
+        <v>153</v>
+      </c>
+      <c r="G33" t="str">
+        <f t="shared" si="2"/>
+        <v>#00</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="3"/>
+        <v>#1F</v>
+      </c>
+      <c r="I33" t="s">
+        <v>3</v>
+      </c>
+      <c r="J33" t="s">
+        <v>37</v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L33" t="str">
+        <f t="shared" si="5"/>
+        <v>#7F</v>
+      </c>
+      <c r="M33" t="s">
+        <v>11</v>
+      </c>
+      <c r="N33" t="s">
+        <v>33</v>
+      </c>
+      <c r="O33" t="str">
+        <f t="shared" si="6"/>
+        <v>#03</v>
+      </c>
+      <c r="P33" t="str">
+        <f t="shared" si="7"/>
+        <v>#E0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fin sprite punto de mira
</commit_message>
<xml_diff>
--- a/doc/diseño sprites/diseno sprites.xlsx
+++ b/doc/diseño sprites/diseno sprites.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="8" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" firstSheet="9" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="zombi" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <sheet name="jefecaballeroi" sheetId="13" r:id="rId13"/>
     <sheet name="jefezombid" sheetId="14" r:id="rId14"/>
     <sheet name="jefezombii" sheetId="15" r:id="rId15"/>
+    <sheet name="punto mira" sheetId="16" r:id="rId16"/>
   </sheets>
   <calcPr calcId="162913" iterateDelta="1E-4"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3202" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3330" uniqueCount="303">
   <si>
     <t>00011111n</t>
   </si>
@@ -8951,7 +8952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P17" sqref="O17:P17"/>
     </sheetView>
   </sheetViews>
@@ -10823,7 +10824,7 @@
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -12682,6 +12683,949 @@
       <c r="P33" t="str">
         <f t="shared" si="7"/>
         <v>#E0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1:P16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(A1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="D1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(B1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(E1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="H1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(F1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(I1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="L1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(J1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="M1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" t="s">
+        <v>3</v>
+      </c>
+      <c r="O1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(M1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="P1" t="str">
+        <f>CONCATENATE("#",BIN2HEX(REPLACE(N1,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C16" si="0">CONCATENATE("#",BIN2HEX(REPLACE(A2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="D2" t="str">
+        <f t="shared" ref="D2:D16" si="1">CONCATENATE("#",BIN2HEX(REPLACE(B2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" t="str">
+        <f t="shared" ref="G2:G16" si="2">CONCATENATE("#",BIN2HEX(REPLACE(E2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="H2" t="str">
+        <f t="shared" ref="H2:H16" si="3">CONCATENATE("#",BIN2HEX(REPLACE(F2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="I2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" t="str">
+        <f t="shared" ref="K2:K16" si="4">CONCATENATE("#",BIN2HEX(REPLACE(I2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="L2" t="str">
+        <f t="shared" ref="L2:L16" si="5">CONCATENATE("#",BIN2HEX(REPLACE(J2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="M2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O2" t="str">
+        <f t="shared" ref="O2:O16" si="6">CONCATENATE("#",BIN2HEX(REPLACE(M2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+      <c r="P2" t="str">
+        <f t="shared" ref="P2:P16" si="7">CONCATENATE("#",BIN2HEX(REPLACE(N2,1,1,""),2))</f>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D3" t="str">
+        <f t="shared" si="1"/>
+        <v>#00</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" si="2"/>
+        <v>#00</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L3" t="str">
+        <f t="shared" si="5"/>
+        <v>#00</v>
+      </c>
+      <c r="M3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" t="s">
+        <v>101</v>
+      </c>
+      <c r="O3" t="str">
+        <f t="shared" si="6"/>
+        <v>#01</v>
+      </c>
+      <c r="P3" t="str">
+        <f t="shared" si="7"/>
+        <v>#80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>#01</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="1"/>
+        <v>#80</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" si="2"/>
+        <v>#02</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" si="3"/>
+        <v>#40</v>
+      </c>
+      <c r="I4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" t="str">
+        <f t="shared" si="4"/>
+        <v>#02</v>
+      </c>
+      <c r="L4" t="str">
+        <f t="shared" si="5"/>
+        <v>#40</v>
+      </c>
+      <c r="M4" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" t="s">
+        <v>101</v>
+      </c>
+      <c r="O4" t="str">
+        <f t="shared" si="6"/>
+        <v>#01</v>
+      </c>
+      <c r="P4" t="str">
+        <f t="shared" si="7"/>
+        <v>#80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>#02</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" si="1"/>
+        <v>#40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>255</v>
+      </c>
+      <c r="F5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="2"/>
+        <v>#05</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="3"/>
+        <v>#A0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K5" t="str">
+        <f t="shared" si="4"/>
+        <v>#04</v>
+      </c>
+      <c r="L5" t="str">
+        <f t="shared" si="5"/>
+        <v>#20</v>
+      </c>
+      <c r="M5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N5" t="s">
+        <v>101</v>
+      </c>
+      <c r="O5" t="str">
+        <f t="shared" si="6"/>
+        <v>#01</v>
+      </c>
+      <c r="P5" t="str">
+        <f t="shared" si="7"/>
+        <v>#80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" t="s">
+        <v>216</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>#04</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" si="1"/>
+        <v>#20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>220</v>
+      </c>
+      <c r="F6" t="s">
+        <v>211</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="2"/>
+        <v>#0B</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="3"/>
+        <v>#D0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>78</v>
+      </c>
+      <c r="J6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K6" t="str">
+        <f t="shared" si="4"/>
+        <v>#0C</v>
+      </c>
+      <c r="L6" t="str">
+        <f t="shared" si="5"/>
+        <v>#30</v>
+      </c>
+      <c r="M6" t="s">
+        <v>11</v>
+      </c>
+      <c r="N6" t="s">
+        <v>76</v>
+      </c>
+      <c r="O6" t="str">
+        <f t="shared" si="6"/>
+        <v>#03</v>
+      </c>
+      <c r="P6" t="str">
+        <f t="shared" si="7"/>
+        <v>#C0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>#01</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="1"/>
+        <v>#80</v>
+      </c>
+      <c r="E7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="2"/>
+        <v>#0E</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="3"/>
+        <v>#70</v>
+      </c>
+      <c r="I7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" t="s">
+        <v>239</v>
+      </c>
+      <c r="K7" t="str">
+        <f t="shared" si="4"/>
+        <v>#12</v>
+      </c>
+      <c r="L7" t="str">
+        <f t="shared" si="5"/>
+        <v>#48</v>
+      </c>
+      <c r="M7" t="s">
+        <v>255</v>
+      </c>
+      <c r="N7" t="s">
+        <v>74</v>
+      </c>
+      <c r="O7" t="str">
+        <f t="shared" si="6"/>
+        <v>#05</v>
+      </c>
+      <c r="P7" t="str">
+        <f t="shared" si="7"/>
+        <v>#A0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" t="s">
+        <v>254</v>
+      </c>
+      <c r="B8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>#0A</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="1"/>
+        <v>#50</v>
+      </c>
+      <c r="E8" t="s">
+        <v>255</v>
+      </c>
+      <c r="F8" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="2"/>
+        <v>#05</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="3"/>
+        <v>#A0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" t="s">
+        <v>101</v>
+      </c>
+      <c r="K8" t="str">
+        <f t="shared" si="4"/>
+        <v>#01</v>
+      </c>
+      <c r="L8" t="str">
+        <f t="shared" si="5"/>
+        <v>#80</v>
+      </c>
+      <c r="M8" t="s">
+        <v>43</v>
+      </c>
+      <c r="N8" t="s">
+        <v>7</v>
+      </c>
+      <c r="O8" t="str">
+        <f t="shared" si="6"/>
+        <v>#3F</v>
+      </c>
+      <c r="P8" t="str">
+        <f t="shared" si="7"/>
+        <v>#FC</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" t="s">
+        <v>254</v>
+      </c>
+      <c r="B9" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>#0A</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="1"/>
+        <v>#50</v>
+      </c>
+      <c r="E9" t="s">
+        <v>255</v>
+      </c>
+      <c r="F9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="2"/>
+        <v>#05</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="3"/>
+        <v>#A0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" t="s">
+        <v>101</v>
+      </c>
+      <c r="K9" t="str">
+        <f t="shared" si="4"/>
+        <v>#01</v>
+      </c>
+      <c r="L9" t="str">
+        <f t="shared" si="5"/>
+        <v>#80</v>
+      </c>
+      <c r="M9" t="s">
+        <v>43</v>
+      </c>
+      <c r="N9" t="s">
+        <v>7</v>
+      </c>
+      <c r="O9" t="str">
+        <f t="shared" si="6"/>
+        <v>#3F</v>
+      </c>
+      <c r="P9" t="str">
+        <f t="shared" si="7"/>
+        <v>#FC</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>#01</v>
+      </c>
+      <c r="D10" t="str">
+        <f t="shared" si="1"/>
+        <v>#80</v>
+      </c>
+      <c r="E10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="2"/>
+        <v>#0E</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="3"/>
+        <v>#70</v>
+      </c>
+      <c r="I10" t="s">
+        <v>47</v>
+      </c>
+      <c r="J10" t="s">
+        <v>239</v>
+      </c>
+      <c r="K10" t="str">
+        <f t="shared" si="4"/>
+        <v>#12</v>
+      </c>
+      <c r="L10" t="str">
+        <f t="shared" si="5"/>
+        <v>#48</v>
+      </c>
+      <c r="M10" t="s">
+        <v>255</v>
+      </c>
+      <c r="N10" t="s">
+        <v>74</v>
+      </c>
+      <c r="O10" t="str">
+        <f t="shared" si="6"/>
+        <v>#05</v>
+      </c>
+      <c r="P10" t="str">
+        <f t="shared" si="7"/>
+        <v>#A0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" t="s">
+        <v>216</v>
+      </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>#04</v>
+      </c>
+      <c r="D11" t="str">
+        <f t="shared" si="1"/>
+        <v>#20</v>
+      </c>
+      <c r="E11" t="s">
+        <v>220</v>
+      </c>
+      <c r="F11" t="s">
+        <v>211</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="2"/>
+        <v>#0B</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="3"/>
+        <v>#D0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>78</v>
+      </c>
+      <c r="J11" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11" t="str">
+        <f t="shared" si="4"/>
+        <v>#0C</v>
+      </c>
+      <c r="L11" t="str">
+        <f t="shared" si="5"/>
+        <v>#30</v>
+      </c>
+      <c r="M11" t="s">
+        <v>11</v>
+      </c>
+      <c r="N11" t="s">
+        <v>76</v>
+      </c>
+      <c r="O11" t="str">
+        <f t="shared" si="6"/>
+        <v>#03</v>
+      </c>
+      <c r="P11" t="str">
+        <f t="shared" si="7"/>
+        <v>#C0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>#02</v>
+      </c>
+      <c r="D12" t="str">
+        <f t="shared" si="1"/>
+        <v>#40</v>
+      </c>
+      <c r="E12" t="s">
+        <v>255</v>
+      </c>
+      <c r="F12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="2"/>
+        <v>#05</v>
+      </c>
+      <c r="H12" t="str">
+        <f t="shared" si="3"/>
+        <v>#A0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>216</v>
+      </c>
+      <c r="J12" t="s">
+        <v>55</v>
+      </c>
+      <c r="K12" t="str">
+        <f t="shared" si="4"/>
+        <v>#04</v>
+      </c>
+      <c r="L12" t="str">
+        <f t="shared" si="5"/>
+        <v>#20</v>
+      </c>
+      <c r="M12" t="s">
+        <v>8</v>
+      </c>
+      <c r="N12" t="s">
+        <v>101</v>
+      </c>
+      <c r="O12" t="str">
+        <f t="shared" si="6"/>
+        <v>#01</v>
+      </c>
+      <c r="P12" t="str">
+        <f t="shared" si="7"/>
+        <v>#80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>#01</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="1"/>
+        <v>#80</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="2"/>
+        <v>#02</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" si="3"/>
+        <v>#40</v>
+      </c>
+      <c r="I13" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" t="s">
+        <v>39</v>
+      </c>
+      <c r="K13" t="str">
+        <f t="shared" si="4"/>
+        <v>#02</v>
+      </c>
+      <c r="L13" t="str">
+        <f t="shared" si="5"/>
+        <v>#40</v>
+      </c>
+      <c r="M13" t="s">
+        <v>8</v>
+      </c>
+      <c r="N13" t="s">
+        <v>101</v>
+      </c>
+      <c r="O13" t="str">
+        <f t="shared" si="6"/>
+        <v>#01</v>
+      </c>
+      <c r="P13" t="str">
+        <f t="shared" si="7"/>
+        <v>#80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="1"/>
+        <v>#00</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" t="str">
+        <f t="shared" si="2"/>
+        <v>#00</v>
+      </c>
+      <c r="H14" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I14" t="s">
+        <v>3</v>
+      </c>
+      <c r="J14" t="s">
+        <v>3</v>
+      </c>
+      <c r="K14" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L14" t="str">
+        <f t="shared" si="5"/>
+        <v>#00</v>
+      </c>
+      <c r="M14" t="s">
+        <v>8</v>
+      </c>
+      <c r="N14" t="s">
+        <v>101</v>
+      </c>
+      <c r="O14" t="str">
+        <f t="shared" si="6"/>
+        <v>#01</v>
+      </c>
+      <c r="P14" t="str">
+        <f t="shared" si="7"/>
+        <v>#80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="1"/>
+        <v>#00</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="2"/>
+        <v>#00</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I15" t="s">
+        <v>3</v>
+      </c>
+      <c r="J15" t="s">
+        <v>3</v>
+      </c>
+      <c r="K15" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L15" t="str">
+        <f t="shared" si="5"/>
+        <v>#00</v>
+      </c>
+      <c r="M15" t="s">
+        <v>3</v>
+      </c>
+      <c r="N15" t="s">
+        <v>3</v>
+      </c>
+      <c r="O15" t="str">
+        <f t="shared" si="6"/>
+        <v>#00</v>
+      </c>
+      <c r="P15" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>#00</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="1"/>
+        <v>#00</v>
+      </c>
+      <c r="E16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" t="str">
+        <f t="shared" si="2"/>
+        <v>#00</v>
+      </c>
+      <c r="H16" t="str">
+        <f t="shared" si="3"/>
+        <v>#00</v>
+      </c>
+      <c r="I16" t="s">
+        <v>3</v>
+      </c>
+      <c r="J16" t="s">
+        <v>3</v>
+      </c>
+      <c r="K16" t="str">
+        <f t="shared" si="4"/>
+        <v>#00</v>
+      </c>
+      <c r="L16" t="str">
+        <f t="shared" si="5"/>
+        <v>#00</v>
+      </c>
+      <c r="M16" t="s">
+        <v>3</v>
+      </c>
+      <c r="N16" t="s">
+        <v>3</v>
+      </c>
+      <c r="O16" t="str">
+        <f t="shared" si="6"/>
+        <v>#00</v>
+      </c>
+      <c r="P16" t="str">
+        <f t="shared" si="7"/>
+        <v>#00</v>
       </c>
     </row>
   </sheetData>

</xml_diff>